<commit_message>
misc updates n sich
</commit_message>
<xml_diff>
--- a/Docs/Excel/HB WO Form.xlsx
+++ b/Docs/Excel/HB WO Form.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\A2\_UX\OnSiteX\Docs\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="A:\_A\_UX\OnSiteX\Docs\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -522,12 +522,30 @@
       <name val="Roboto Condensed"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="11">
@@ -646,7 +664,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="83">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -685,12 +703,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -700,161 +712,203 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1141,8 +1195,8 @@
   </sheetPr>
   <dimension ref="A1:O48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42:O48"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K34" sqref="K34:O34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.3"/>
@@ -1163,70 +1217,70 @@
   <sheetData>
     <row r="1" spans="1:15" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="1:15" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="69"/>
-      <c r="J2" s="33" t="s">
+      <c r="C2" s="17"/>
+      <c r="D2" s="17"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="22" t="s">
         <v>99</v>
       </c>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="70"/>
-      <c r="N2" s="50"/>
-      <c r="O2" s="51"/>
+      <c r="K2" s="18"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="18"/>
+      <c r="N2" s="19"/>
+      <c r="O2" s="20"/>
     </row>
     <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="14"/>
-      <c r="B3" s="15" t="s">
+      <c r="A3" s="27"/>
+      <c r="B3" s="28" t="s">
         <v>93</v>
       </c>
-      <c r="C3" s="34" t="s">
+      <c r="C3" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="35"/>
-      <c r="G3" s="34" t="s">
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="33"/>
+      <c r="G3" s="31" t="s">
         <v>95</v>
       </c>
-      <c r="H3" s="42"/>
-      <c r="I3" s="35"/>
-      <c r="J3" s="55" t="s">
+      <c r="H3" s="32"/>
+      <c r="I3" s="33"/>
+      <c r="J3" s="34" t="s">
         <v>96</v>
       </c>
-      <c r="K3" s="56"/>
-      <c r="L3" s="34" t="s">
+      <c r="K3" s="35"/>
+      <c r="L3" s="31" t="s">
         <v>97</v>
       </c>
-      <c r="M3" s="42"/>
-      <c r="N3" s="34" t="s">
+      <c r="M3" s="32"/>
+      <c r="N3" s="31" t="s">
         <v>98</v>
       </c>
-      <c r="O3" s="35"/>
+      <c r="O3" s="33"/>
     </row>
     <row r="4" spans="1:15" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="36"/>
-      <c r="B4" s="37"/>
-      <c r="C4" s="36"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="41"/>
-      <c r="I4" s="37"/>
-      <c r="J4" s="36"/>
-      <c r="K4" s="37"/>
-      <c r="L4" s="36"/>
-      <c r="M4" s="41"/>
-      <c r="N4" s="36"/>
-      <c r="O4" s="37"/>
+      <c r="A4" s="29"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="25"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="26"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="26"/>
+      <c r="J4" s="25"/>
+      <c r="K4" s="26"/>
+      <c r="L4" s="25"/>
+      <c r="M4" s="36"/>
+      <c r="N4" s="25"/>
+      <c r="O4" s="26"/>
     </row>
     <row r="5" spans="1:15" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="12"/>
@@ -1246,1122 +1300,1143 @@
       <c r="O5" s="9"/>
     </row>
     <row r="6" spans="1:15" s="13" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="31"/>
-      <c r="B6" s="59" t="s">
+      <c r="A6" s="37"/>
+      <c r="B6" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="C6" s="59"/>
-      <c r="D6" s="59"/>
-      <c r="E6" s="60"/>
-      <c r="F6" s="32" t="s">
-        <v>54</v>
-      </c>
-      <c r="G6" s="50" t="s">
+      <c r="C6" s="38"/>
+      <c r="D6" s="38"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="40" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" s="41" t="s">
         <v>83</v>
       </c>
-      <c r="H6" s="50"/>
-      <c r="I6" s="51"/>
-      <c r="J6" s="61" t="s">
+      <c r="H6" s="41"/>
+      <c r="I6" s="42"/>
+      <c r="J6" s="43" t="s">
         <v>126</v>
       </c>
-      <c r="K6" s="62"/>
-      <c r="L6" s="65"/>
-      <c r="M6" s="65"/>
-      <c r="N6" s="65"/>
-      <c r="O6" s="66"/>
+      <c r="K6" s="44"/>
+      <c r="L6" s="45"/>
+      <c r="M6" s="45"/>
+      <c r="N6" s="45"/>
+      <c r="O6" s="46"/>
     </row>
     <row r="7" spans="1:15" s="13" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="52"/>
-      <c r="B7" s="53"/>
-      <c r="C7" s="53"/>
-      <c r="D7" s="53"/>
-      <c r="E7" s="54"/>
-      <c r="F7" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="G7" s="57" t="s">
+      <c r="A7" s="47"/>
+      <c r="B7" s="48"/>
+      <c r="C7" s="48"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="50" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" s="51" t="s">
         <v>86</v>
       </c>
-      <c r="H7" s="57"/>
-      <c r="I7" s="58"/>
-      <c r="J7" s="63"/>
-      <c r="K7" s="64"/>
-      <c r="L7" s="67"/>
-      <c r="M7" s="67"/>
-      <c r="N7" s="67"/>
-      <c r="O7" s="68"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="52"/>
+      <c r="J7" s="53"/>
+      <c r="K7" s="54"/>
+      <c r="L7" s="55"/>
+      <c r="M7" s="55"/>
+      <c r="N7" s="55"/>
+      <c r="O7" s="56"/>
     </row>
     <row r="8" spans="1:15" s="13" customFormat="1" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="16"/>
-      <c r="B8" s="16"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
       <c r="F8" s="11"/>
       <c r="G8" s="11"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
       <c r="J8" s="12"/>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="18"/>
-      <c r="N8" s="18"/>
-      <c r="O8" s="18"/>
+      <c r="K8" s="16"/>
+      <c r="L8" s="16"/>
+      <c r="M8" s="16"/>
+      <c r="N8" s="16"/>
+      <c r="O8" s="16"/>
     </row>
     <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="49" t="s">
+      <c r="A9" s="78" t="s">
         <v>128</v>
       </c>
-      <c r="B9" s="50"/>
-      <c r="C9" s="51"/>
-      <c r="D9" s="49" t="s">
+      <c r="B9" s="79"/>
+      <c r="C9" s="80"/>
+      <c r="D9" s="78" t="s">
         <v>130</v>
       </c>
-      <c r="E9" s="50"/>
-      <c r="F9" s="50"/>
-      <c r="G9" s="25"/>
-      <c r="H9" s="49" t="s">
+      <c r="E9" s="79"/>
+      <c r="F9" s="79"/>
+      <c r="G9" s="81"/>
+      <c r="H9" s="78" t="s">
         <v>129</v>
       </c>
-      <c r="I9" s="50"/>
-      <c r="J9" s="51"/>
-      <c r="K9" s="49" t="s">
+      <c r="I9" s="79"/>
+      <c r="J9" s="80"/>
+      <c r="K9" s="78" t="s">
         <v>131</v>
       </c>
-      <c r="L9" s="50"/>
-      <c r="M9" s="50"/>
-      <c r="N9" s="50"/>
-      <c r="O9" s="51"/>
+      <c r="L9" s="79"/>
+      <c r="M9" s="79"/>
+      <c r="N9" s="79"/>
+      <c r="O9" s="80"/>
     </row>
     <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="19"/>
-      <c r="B10" s="9" t="s">
+      <c r="A10" s="58"/>
+      <c r="B10" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="20"/>
-      <c r="D10" s="23"/>
-      <c r="E10" s="9" t="s">
+      <c r="C10" s="60"/>
+      <c r="D10" s="64"/>
+      <c r="E10" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="F10" s="9"/>
-      <c r="G10" s="20"/>
-      <c r="H10" s="23"/>
-      <c r="I10" s="9" t="s">
+      <c r="F10" s="59"/>
+      <c r="G10" s="60"/>
+      <c r="H10" s="64"/>
+      <c r="I10" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="J10" s="20"/>
-      <c r="K10" s="23"/>
-      <c r="L10" s="9" t="s">
+      <c r="J10" s="60"/>
+      <c r="K10" s="64"/>
+      <c r="L10" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="M10" s="9"/>
-      <c r="N10" s="9"/>
-      <c r="O10" s="20"/>
+      <c r="M10" s="59"/>
+      <c r="N10" s="59"/>
+      <c r="O10" s="60"/>
     </row>
     <row r="11" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="B11" s="9" t="s">
+      <c r="A11" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="59" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="20"/>
-      <c r="D11" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="E11" s="9" t="s">
+      <c r="C11" s="60"/>
+      <c r="D11" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="59" t="s">
         <v>112</v>
       </c>
-      <c r="F11" s="9"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="I11" s="9" t="s">
+      <c r="F11" s="59"/>
+      <c r="G11" s="60"/>
+      <c r="H11" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="I11" s="59" t="s">
         <v>56</v>
       </c>
-      <c r="J11" s="20"/>
-      <c r="K11" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="L11" s="9" t="s">
+      <c r="J11" s="60"/>
+      <c r="K11" s="65" t="s">
+        <v>54</v>
+      </c>
+      <c r="L11" s="59" t="s">
         <v>49</v>
       </c>
-      <c r="M11" s="9"/>
-      <c r="N11" s="9"/>
-      <c r="O11" s="20"/>
+      <c r="M11" s="59"/>
+      <c r="N11" s="59"/>
+      <c r="O11" s="60"/>
     </row>
     <row r="12" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="B12" s="9" t="s">
+      <c r="A12" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="20"/>
-      <c r="D12" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="E12" s="9" t="s">
+      <c r="C12" s="60"/>
+      <c r="D12" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="59" t="s">
         <v>113</v>
       </c>
-      <c r="F12" s="9"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="I12" s="9" t="s">
+      <c r="F12" s="59"/>
+      <c r="G12" s="60"/>
+      <c r="H12" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="I12" s="59" t="s">
         <v>57</v>
       </c>
-      <c r="J12" s="20"/>
-      <c r="K12" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="L12" s="9" t="s">
+      <c r="J12" s="60"/>
+      <c r="K12" s="65" t="s">
+        <v>54</v>
+      </c>
+      <c r="L12" s="59" t="s">
         <v>50</v>
       </c>
-      <c r="M12" s="9"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="20"/>
+      <c r="M12" s="59"/>
+      <c r="N12" s="59"/>
+      <c r="O12" s="60"/>
     </row>
     <row r="13" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="B13" s="9" t="s">
+      <c r="A13" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="59" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="20"/>
-      <c r="D13" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="E13" s="9" t="s">
+      <c r="C13" s="60"/>
+      <c r="D13" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="59" t="s">
         <v>114</v>
       </c>
-      <c r="F13" s="9"/>
-      <c r="G13" s="20"/>
-      <c r="H13" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="I13" s="9" t="s">
+      <c r="F13" s="59"/>
+      <c r="G13" s="60"/>
+      <c r="H13" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="I13" s="59" t="s">
         <v>58</v>
       </c>
-      <c r="J13" s="20"/>
-      <c r="K13" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="L13" s="9" t="s">
+      <c r="J13" s="60"/>
+      <c r="K13" s="65" t="s">
+        <v>54</v>
+      </c>
+      <c r="L13" s="59" t="s">
         <v>51</v>
       </c>
-      <c r="M13" s="9"/>
-      <c r="N13" s="9"/>
-      <c r="O13" s="20"/>
+      <c r="M13" s="59"/>
+      <c r="N13" s="59"/>
+      <c r="O13" s="60"/>
     </row>
     <row r="14" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="B14" s="9" t="s">
+      <c r="A14" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="20"/>
-      <c r="D14" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="E14" s="9" t="s">
+      <c r="C14" s="60"/>
+      <c r="D14" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="59" t="s">
         <v>115</v>
       </c>
-      <c r="F14" s="9"/>
-      <c r="G14" s="20"/>
-      <c r="H14" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="I14" s="9" t="s">
+      <c r="F14" s="59"/>
+      <c r="G14" s="60"/>
+      <c r="H14" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="I14" s="59" t="s">
         <v>59</v>
       </c>
-      <c r="J14" s="20"/>
-      <c r="K14" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="L14" s="9" t="s">
+      <c r="J14" s="60"/>
+      <c r="K14" s="65" t="s">
+        <v>54</v>
+      </c>
+      <c r="L14" s="59" t="s">
         <v>52</v>
       </c>
-      <c r="M14" s="9"/>
-      <c r="N14" s="9"/>
-      <c r="O14" s="20"/>
+      <c r="M14" s="59"/>
+      <c r="N14" s="59"/>
+      <c r="O14" s="60"/>
     </row>
     <row r="15" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="B15" s="9" t="s">
+      <c r="A15" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="20"/>
-      <c r="D15" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="E15" s="9" t="s">
+      <c r="C15" s="60"/>
+      <c r="D15" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="59" t="s">
         <v>116</v>
       </c>
-      <c r="F15" s="9"/>
-      <c r="G15" s="20"/>
-      <c r="H15" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="I15" s="9" t="s">
+      <c r="F15" s="59"/>
+      <c r="G15" s="60"/>
+      <c r="H15" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="I15" s="59" t="s">
         <v>60</v>
       </c>
-      <c r="J15" s="20"/>
-      <c r="K15" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="L15" s="9" t="s">
+      <c r="J15" s="60"/>
+      <c r="K15" s="65" t="s">
+        <v>54</v>
+      </c>
+      <c r="L15" s="59" t="s">
         <v>53</v>
       </c>
-      <c r="M15" s="9"/>
-      <c r="N15" s="9"/>
-      <c r="O15" s="20"/>
+      <c r="M15" s="59"/>
+      <c r="N15" s="59"/>
+      <c r="O15" s="60"/>
     </row>
     <row r="16" spans="1:15" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="B16" s="9" t="s">
+      <c r="A16" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="59" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="20"/>
-      <c r="D16" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="E16" s="9" t="s">
+      <c r="C16" s="60"/>
+      <c r="D16" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="59" t="s">
         <v>117</v>
       </c>
-      <c r="F16" s="9"/>
-      <c r="G16" s="20"/>
-      <c r="H16" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="I16" s="9" t="s">
+      <c r="F16" s="59"/>
+      <c r="G16" s="60"/>
+      <c r="H16" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="I16" s="59" t="s">
         <v>61</v>
       </c>
-      <c r="J16" s="20"/>
-      <c r="K16" s="23"/>
-      <c r="L16" s="9" t="s">
+      <c r="J16" s="60"/>
+      <c r="K16" s="64"/>
+      <c r="L16" s="59" t="s">
         <v>125</v>
       </c>
-      <c r="M16" s="9"/>
-      <c r="N16" s="9"/>
-      <c r="O16" s="20"/>
+      <c r="M16" s="59"/>
+      <c r="N16" s="59"/>
+      <c r="O16" s="60"/>
     </row>
     <row r="17" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="B17" s="9" t="s">
+      <c r="A17" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="20"/>
-      <c r="D17" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="E17" s="9" t="s">
+      <c r="C17" s="60"/>
+      <c r="D17" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" s="59" t="s">
         <v>118</v>
       </c>
-      <c r="F17" s="9"/>
-      <c r="G17" s="20"/>
-      <c r="H17" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="I17" s="9" t="s">
+      <c r="F17" s="59"/>
+      <c r="G17" s="60"/>
+      <c r="H17" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="I17" s="59" t="s">
         <v>62</v>
       </c>
-      <c r="J17" s="9"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="26"/>
-      <c r="M17" s="26"/>
-      <c r="N17" s="26"/>
-      <c r="O17" s="15"/>
+      <c r="J17" s="59"/>
+      <c r="K17" s="23"/>
+      <c r="L17" s="66"/>
+      <c r="M17" s="66"/>
+      <c r="N17" s="66"/>
+      <c r="O17" s="24"/>
     </row>
     <row r="18" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="B18" s="9" t="s">
+      <c r="A18" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="59" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="20"/>
-      <c r="D18" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="E18" s="9" t="s">
+      <c r="C18" s="60"/>
+      <c r="D18" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" s="59" t="s">
         <v>119</v>
       </c>
-      <c r="F18" s="9"/>
-      <c r="G18" s="20"/>
-      <c r="H18" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="I18" s="9" t="s">
+      <c r="F18" s="59"/>
+      <c r="G18" s="60"/>
+      <c r="H18" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="I18" s="59" t="s">
         <v>63</v>
       </c>
-      <c r="J18" s="9"/>
-      <c r="K18" s="23"/>
-      <c r="L18" s="9" t="s">
+      <c r="J18" s="59"/>
+      <c r="K18" s="64"/>
+      <c r="L18" s="82" t="s">
         <v>75</v>
       </c>
-      <c r="M18" s="9"/>
-      <c r="N18" s="9"/>
-      <c r="O18" s="20"/>
+      <c r="M18" s="82"/>
+      <c r="N18" s="59"/>
+      <c r="O18" s="60"/>
     </row>
     <row r="19" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="B19" s="9" t="s">
+      <c r="A19" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="20"/>
-      <c r="D19" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="E19" s="9" t="s">
+      <c r="C19" s="60"/>
+      <c r="D19" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" s="59" t="s">
         <v>120</v>
       </c>
-      <c r="F19" s="9"/>
-      <c r="G19" s="20"/>
-      <c r="H19" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="I19" s="9" t="s">
+      <c r="F19" s="59"/>
+      <c r="G19" s="60"/>
+      <c r="H19" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="I19" s="59" t="s">
         <v>64</v>
       </c>
-      <c r="J19" s="9"/>
-      <c r="K19" s="23"/>
-      <c r="L19" s="9" t="s">
+      <c r="J19" s="59"/>
+      <c r="K19" s="64"/>
+      <c r="L19" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="M19" s="9"/>
-      <c r="N19" s="9"/>
-      <c r="O19" s="20"/>
+      <c r="M19" s="59"/>
+      <c r="N19" s="59"/>
+      <c r="O19" s="60"/>
     </row>
     <row r="20" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="B20" s="9" t="s">
+      <c r="A20" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="20"/>
-      <c r="D20" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="E20" s="9" t="s">
+      <c r="C20" s="60"/>
+      <c r="D20" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="E20" s="59" t="s">
         <v>121</v>
       </c>
-      <c r="F20" s="9"/>
-      <c r="G20" s="20"/>
-      <c r="H20" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="I20" s="9" t="s">
+      <c r="F20" s="59"/>
+      <c r="G20" s="60"/>
+      <c r="H20" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="I20" s="59" t="s">
         <v>65</v>
       </c>
-      <c r="J20" s="9"/>
-      <c r="K20" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="L20" s="9" t="s">
+      <c r="J20" s="59"/>
+      <c r="K20" s="65" t="s">
+        <v>54</v>
+      </c>
+      <c r="L20" s="59" t="s">
         <v>76</v>
       </c>
-      <c r="M20" s="9"/>
-      <c r="N20" s="9"/>
-      <c r="O20" s="20"/>
+      <c r="M20" s="59"/>
+      <c r="N20" s="59"/>
+      <c r="O20" s="60"/>
     </row>
     <row r="21" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="B21" s="9" t="s">
+      <c r="A21" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="20"/>
-      <c r="D21" s="23"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="20"/>
-      <c r="H21" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="I21" s="9" t="s">
+      <c r="C21" s="60"/>
+      <c r="D21" s="64"/>
+      <c r="E21" s="59"/>
+      <c r="F21" s="59"/>
+      <c r="G21" s="60"/>
+      <c r="H21" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="I21" s="59" t="s">
         <v>66</v>
       </c>
-      <c r="J21" s="9"/>
-      <c r="K21" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="L21" s="9" t="s">
+      <c r="J21" s="59"/>
+      <c r="K21" s="65" t="s">
+        <v>54</v>
+      </c>
+      <c r="L21" s="59" t="s">
         <v>77</v>
       </c>
-      <c r="M21" s="9"/>
-      <c r="N21" s="9"/>
-      <c r="O21" s="20"/>
+      <c r="M21" s="59"/>
+      <c r="N21" s="59"/>
+      <c r="O21" s="60"/>
     </row>
     <row r="22" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="B22" s="9" t="s">
+      <c r="A22" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" s="59" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="20"/>
-      <c r="D22" s="23"/>
-      <c r="E22" s="9"/>
-      <c r="F22" s="9"/>
-      <c r="G22" s="20"/>
-      <c r="H22" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="I22" s="9" t="s">
+      <c r="C22" s="60"/>
+      <c r="D22" s="64"/>
+      <c r="E22" s="59"/>
+      <c r="F22" s="59"/>
+      <c r="G22" s="60"/>
+      <c r="H22" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="I22" s="59" t="s">
         <v>67</v>
       </c>
-      <c r="J22" s="9"/>
-      <c r="K22" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="L22" s="9" t="s">
+      <c r="J22" s="59"/>
+      <c r="K22" s="65" t="s">
+        <v>54</v>
+      </c>
+      <c r="L22" s="59" t="s">
         <v>78</v>
       </c>
-      <c r="M22" s="9"/>
-      <c r="N22" s="9"/>
-      <c r="O22" s="20"/>
+      <c r="M22" s="59"/>
+      <c r="N22" s="59"/>
+      <c r="O22" s="60"/>
     </row>
     <row r="23" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="B23" s="9" t="s">
+      <c r="A23" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="59" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="20"/>
-      <c r="D23" s="23"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="I23" s="9" t="s">
+      <c r="C23" s="60"/>
+      <c r="D23" s="64"/>
+      <c r="E23" s="59"/>
+      <c r="F23" s="59"/>
+      <c r="G23" s="60"/>
+      <c r="H23" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="I23" s="59" t="s">
         <v>68</v>
       </c>
-      <c r="J23" s="9"/>
-      <c r="K23" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="L23" s="9" t="s">
+      <c r="J23" s="59"/>
+      <c r="K23" s="65" t="s">
+        <v>54</v>
+      </c>
+      <c r="L23" s="59" t="s">
         <v>79</v>
       </c>
-      <c r="M23" s="9"/>
-      <c r="N23" s="9"/>
-      <c r="O23" s="20"/>
+      <c r="M23" s="59"/>
+      <c r="N23" s="59"/>
+      <c r="O23" s="60"/>
     </row>
     <row r="24" spans="1:15" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="B24" s="9" t="s">
+      <c r="A24" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="59" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="20"/>
-      <c r="D24" s="23"/>
-      <c r="E24" s="9"/>
-      <c r="F24" s="9"/>
-      <c r="G24" s="20"/>
-      <c r="H24" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="I24" s="9" t="s">
+      <c r="C24" s="60"/>
+      <c r="D24" s="64"/>
+      <c r="E24" s="59"/>
+      <c r="F24" s="59"/>
+      <c r="G24" s="60"/>
+      <c r="H24" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="I24" s="59" t="s">
         <v>69</v>
       </c>
-      <c r="J24" s="9"/>
-      <c r="K24" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="L24" s="21" t="s">
+      <c r="J24" s="59"/>
+      <c r="K24" s="67" t="s">
+        <v>54</v>
+      </c>
+      <c r="L24" s="62" t="s">
         <v>80</v>
       </c>
-      <c r="M24" s="21"/>
-      <c r="N24" s="21"/>
-      <c r="O24" s="22"/>
+      <c r="M24" s="62"/>
+      <c r="N24" s="62"/>
+      <c r="O24" s="63"/>
     </row>
     <row r="25" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="B25" s="9" t="s">
+      <c r="A25" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="59" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="20"/>
-      <c r="D25" s="23"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="I25" s="9" t="s">
+      <c r="C25" s="60"/>
+      <c r="D25" s="64"/>
+      <c r="E25" s="59"/>
+      <c r="F25" s="59"/>
+      <c r="G25" s="60"/>
+      <c r="H25" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="I25" s="59" t="s">
         <v>70</v>
       </c>
-      <c r="J25" s="9"/>
-      <c r="K25" s="34" t="s">
+      <c r="J25" s="59"/>
+      <c r="K25" s="31" t="s">
         <v>122</v>
       </c>
-      <c r="L25" s="42"/>
-      <c r="M25" s="35"/>
-      <c r="N25" s="34" t="s">
+      <c r="L25" s="32"/>
+      <c r="M25" s="33"/>
+      <c r="N25" s="31" t="s">
         <v>134</v>
       </c>
-      <c r="O25" s="35"/>
+      <c r="O25" s="33"/>
     </row>
     <row r="26" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="B26" s="9" t="s">
+      <c r="A26" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" s="59" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="20"/>
-      <c r="D26" s="23"/>
-      <c r="E26" s="9"/>
-      <c r="F26" s="9"/>
-      <c r="G26" s="20"/>
-      <c r="H26" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="I26" s="9" t="s">
+      <c r="C26" s="60"/>
+      <c r="D26" s="64"/>
+      <c r="E26" s="59"/>
+      <c r="F26" s="59"/>
+      <c r="G26" s="60"/>
+      <c r="H26" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="I26" s="59" t="s">
         <v>71</v>
       </c>
-      <c r="J26" s="9"/>
-      <c r="K26" s="38"/>
-      <c r="L26" s="39"/>
-      <c r="M26" s="40"/>
-      <c r="N26" s="38"/>
-      <c r="O26" s="40"/>
+      <c r="J26" s="59"/>
+      <c r="K26" s="68"/>
+      <c r="L26" s="69"/>
+      <c r="M26" s="70"/>
+      <c r="N26" s="68"/>
+      <c r="O26" s="70"/>
     </row>
     <row r="27" spans="1:15" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="B27" s="9" t="s">
+      <c r="A27" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="59" t="s">
         <v>18</v>
       </c>
-      <c r="C27" s="20"/>
-      <c r="D27" s="23"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="I27" s="9" t="s">
+      <c r="C27" s="60"/>
+      <c r="D27" s="64"/>
+      <c r="E27" s="59"/>
+      <c r="F27" s="59"/>
+      <c r="G27" s="60"/>
+      <c r="H27" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="I27" s="59" t="s">
         <v>72</v>
       </c>
-      <c r="J27" s="9"/>
-      <c r="K27" s="36"/>
-      <c r="L27" s="41"/>
-      <c r="M27" s="37"/>
-      <c r="N27" s="36"/>
-      <c r="O27" s="37"/>
+      <c r="J27" s="59"/>
+      <c r="K27" s="25"/>
+      <c r="L27" s="36"/>
+      <c r="M27" s="26"/>
+      <c r="N27" s="25"/>
+      <c r="O27" s="26"/>
     </row>
     <row r="28" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="B28" s="9" t="s">
+      <c r="A28" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="59" t="s">
         <v>19</v>
       </c>
-      <c r="C28" s="20"/>
-      <c r="D28" s="23"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="20"/>
-      <c r="H28" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="I28" s="9" t="s">
+      <c r="C28" s="60"/>
+      <c r="D28" s="64"/>
+      <c r="E28" s="59"/>
+      <c r="F28" s="59"/>
+      <c r="G28" s="60"/>
+      <c r="H28" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="I28" s="59" t="s">
         <v>73</v>
       </c>
-      <c r="J28" s="9"/>
-      <c r="K28" s="34" t="s">
+      <c r="J28" s="59"/>
+      <c r="K28" s="31" t="s">
         <v>124</v>
       </c>
-      <c r="L28" s="42"/>
-      <c r="M28" s="42"/>
-      <c r="N28" s="42"/>
-      <c r="O28" s="35"/>
+      <c r="L28" s="32"/>
+      <c r="M28" s="32"/>
+      <c r="N28" s="32"/>
+      <c r="O28" s="33"/>
     </row>
     <row r="29" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="B29" s="9" t="s">
+      <c r="A29" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" s="59" t="s">
         <v>20</v>
       </c>
-      <c r="C29" s="20"/>
-      <c r="D29" s="23"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="20"/>
-      <c r="H29" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="I29" s="9" t="s">
+      <c r="C29" s="60"/>
+      <c r="D29" s="64"/>
+      <c r="E29" s="59"/>
+      <c r="F29" s="59"/>
+      <c r="G29" s="60"/>
+      <c r="H29" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="I29" s="59" t="s">
         <v>74</v>
       </c>
-      <c r="J29" s="20"/>
-      <c r="K29" s="38"/>
-      <c r="L29" s="39"/>
-      <c r="M29" s="39"/>
-      <c r="N29" s="39"/>
-      <c r="O29" s="40"/>
+      <c r="J29" s="60"/>
+      <c r="K29" s="68"/>
+      <c r="L29" s="69"/>
+      <c r="M29" s="69"/>
+      <c r="N29" s="69"/>
+      <c r="O29" s="70"/>
     </row>
     <row r="30" spans="1:15" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="B30" s="9" t="s">
+      <c r="A30" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="C30" s="20"/>
-      <c r="D30" s="24"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="21"/>
-      <c r="G30" s="22"/>
-      <c r="H30" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="I30" s="21" t="s">
+      <c r="C30" s="60"/>
+      <c r="D30" s="71"/>
+      <c r="E30" s="62"/>
+      <c r="F30" s="62"/>
+      <c r="G30" s="63"/>
+      <c r="H30" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="I30" s="62" t="s">
         <v>37</v>
       </c>
-      <c r="J30" s="22"/>
-      <c r="K30" s="36"/>
-      <c r="L30" s="41"/>
-      <c r="M30" s="41"/>
-      <c r="N30" s="41"/>
-      <c r="O30" s="37"/>
+      <c r="J30" s="63"/>
+      <c r="K30" s="25"/>
+      <c r="L30" s="36"/>
+      <c r="M30" s="36"/>
+      <c r="N30" s="36"/>
+      <c r="O30" s="26"/>
     </row>
     <row r="31" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="B31" s="9" t="s">
+      <c r="A31" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="B31" s="59" t="s">
         <v>22</v>
       </c>
-      <c r="C31" s="20"/>
-      <c r="D31" s="49" t="s">
+      <c r="C31" s="60"/>
+      <c r="D31" s="57" t="s">
         <v>100</v>
       </c>
-      <c r="E31" s="50"/>
-      <c r="F31" s="50"/>
-      <c r="G31" s="50"/>
-      <c r="H31" s="50"/>
-      <c r="I31" s="50"/>
-      <c r="J31" s="51"/>
-      <c r="K31" s="49" t="s">
+      <c r="E31" s="19"/>
+      <c r="F31" s="19"/>
+      <c r="G31" s="19"/>
+      <c r="H31" s="19"/>
+      <c r="I31" s="19"/>
+      <c r="J31" s="20"/>
+      <c r="K31" s="78" t="s">
         <v>133</v>
       </c>
-      <c r="L31" s="50"/>
-      <c r="M31" s="50"/>
-      <c r="N31" s="50"/>
-      <c r="O31" s="51"/>
+      <c r="L31" s="79"/>
+      <c r="M31" s="79"/>
+      <c r="N31" s="79"/>
+      <c r="O31" s="80"/>
     </row>
     <row r="32" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="B32" s="9" t="s">
+      <c r="A32" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="B32" s="59" t="s">
         <v>81</v>
       </c>
-      <c r="C32" s="20"/>
-      <c r="D32" s="38"/>
-      <c r="E32" s="39"/>
-      <c r="F32" s="39"/>
-      <c r="G32" s="39"/>
-      <c r="H32" s="39"/>
-      <c r="I32" s="39"/>
-      <c r="J32" s="40"/>
-      <c r="K32" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="L32" s="9" t="s">
+      <c r="C32" s="60"/>
+      <c r="D32" s="68"/>
+      <c r="E32" s="69"/>
+      <c r="F32" s="69"/>
+      <c r="G32" s="69"/>
+      <c r="H32" s="69"/>
+      <c r="I32" s="69"/>
+      <c r="J32" s="70"/>
+      <c r="K32" s="65" t="s">
+        <v>54</v>
+      </c>
+      <c r="L32" s="59" t="s">
         <v>102</v>
       </c>
-      <c r="M32" s="9"/>
-      <c r="N32" s="9"/>
-      <c r="O32" s="20"/>
+      <c r="M32" s="59"/>
+      <c r="N32" s="59"/>
+      <c r="O32" s="60"/>
     </row>
     <row r="33" spans="1:15" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="B33" s="9" t="s">
+      <c r="A33" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="B33" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="20"/>
-      <c r="D33" s="38"/>
-      <c r="E33" s="39"/>
-      <c r="F33" s="39"/>
-      <c r="G33" s="39"/>
-      <c r="H33" s="39"/>
-      <c r="I33" s="39"/>
-      <c r="J33" s="40"/>
-      <c r="K33" s="24"/>
-      <c r="L33" s="21"/>
-      <c r="M33" s="21"/>
-      <c r="N33" s="21"/>
-      <c r="O33" s="22"/>
+      <c r="C33" s="60"/>
+      <c r="D33" s="68"/>
+      <c r="E33" s="69"/>
+      <c r="F33" s="69"/>
+      <c r="G33" s="69"/>
+      <c r="H33" s="69"/>
+      <c r="I33" s="69"/>
+      <c r="J33" s="70"/>
+      <c r="K33" s="71"/>
+      <c r="L33" s="62"/>
+      <c r="M33" s="62"/>
+      <c r="N33" s="62"/>
+      <c r="O33" s="63"/>
     </row>
     <row r="34" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="B34" s="9" t="s">
+      <c r="A34" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34" s="59" t="s">
         <v>25</v>
       </c>
-      <c r="C34" s="20"/>
-      <c r="D34" s="38"/>
-      <c r="E34" s="39"/>
-      <c r="F34" s="39"/>
-      <c r="G34" s="39"/>
-      <c r="H34" s="39"/>
-      <c r="I34" s="39"/>
-      <c r="J34" s="40"/>
-      <c r="K34" s="49" t="s">
+      <c r="C34" s="60"/>
+      <c r="D34" s="68"/>
+      <c r="E34" s="69"/>
+      <c r="F34" s="69"/>
+      <c r="G34" s="69"/>
+      <c r="H34" s="69"/>
+      <c r="I34" s="69"/>
+      <c r="J34" s="70"/>
+      <c r="K34" s="78" t="s">
         <v>132</v>
       </c>
-      <c r="L34" s="50"/>
-      <c r="M34" s="50"/>
-      <c r="N34" s="50"/>
-      <c r="O34" s="51"/>
+      <c r="L34" s="79"/>
+      <c r="M34" s="79"/>
+      <c r="N34" s="79"/>
+      <c r="O34" s="80"/>
     </row>
     <row r="35" spans="1:15" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="B35" s="9" t="s">
+      <c r="A35" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="B35" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="C35" s="20"/>
-      <c r="D35" s="36"/>
-      <c r="E35" s="41"/>
-      <c r="F35" s="41"/>
-      <c r="G35" s="41"/>
-      <c r="H35" s="41"/>
-      <c r="I35" s="41"/>
-      <c r="J35" s="37"/>
-      <c r="K35" s="23"/>
-      <c r="L35" s="9" t="s">
+      <c r="C35" s="60"/>
+      <c r="D35" s="25"/>
+      <c r="E35" s="36"/>
+      <c r="F35" s="36"/>
+      <c r="G35" s="36"/>
+      <c r="H35" s="36"/>
+      <c r="I35" s="36"/>
+      <c r="J35" s="26"/>
+      <c r="K35" s="64"/>
+      <c r="L35" s="59" t="s">
         <v>1</v>
       </c>
-      <c r="M35" s="9"/>
-      <c r="N35" s="9"/>
-      <c r="O35" s="20"/>
+      <c r="M35" s="59"/>
+      <c r="N35" s="59"/>
+      <c r="O35" s="60"/>
     </row>
     <row r="36" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="B36" s="9" t="s">
+      <c r="A36" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="B36" s="59" t="s">
         <v>41</v>
       </c>
-      <c r="C36" s="20"/>
-      <c r="D36" s="49" t="s">
+      <c r="C36" s="60"/>
+      <c r="D36" s="57" t="s">
         <v>101</v>
       </c>
-      <c r="E36" s="50"/>
-      <c r="F36" s="50"/>
-      <c r="G36" s="50"/>
-      <c r="H36" s="50"/>
-      <c r="I36" s="50"/>
-      <c r="J36" s="51"/>
-      <c r="K36" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="L36" s="9" t="s">
+      <c r="E36" s="19"/>
+      <c r="F36" s="19"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="19"/>
+      <c r="I36" s="19"/>
+      <c r="J36" s="20"/>
+      <c r="K36" s="65" t="s">
+        <v>54</v>
+      </c>
+      <c r="L36" s="59" t="s">
         <v>109</v>
       </c>
-      <c r="M36" s="9"/>
-      <c r="N36" s="9"/>
-      <c r="O36" s="20"/>
+      <c r="M36" s="59"/>
+      <c r="N36" s="59"/>
+      <c r="O36" s="60"/>
     </row>
     <row r="37" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="B37" s="9" t="s">
+      <c r="A37" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="B37" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="C37" s="20"/>
-      <c r="D37" s="38"/>
-      <c r="E37" s="39"/>
-      <c r="F37" s="39"/>
-      <c r="G37" s="39"/>
-      <c r="H37" s="39"/>
-      <c r="I37" s="39"/>
-      <c r="J37" s="40"/>
-      <c r="K37" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="L37" s="9" t="s">
+      <c r="C37" s="60"/>
+      <c r="D37" s="68"/>
+      <c r="E37" s="69"/>
+      <c r="F37" s="69"/>
+      <c r="G37" s="69"/>
+      <c r="H37" s="69"/>
+      <c r="I37" s="69"/>
+      <c r="J37" s="70"/>
+      <c r="K37" s="65" t="s">
+        <v>54</v>
+      </c>
+      <c r="L37" s="59" t="s">
         <v>104</v>
       </c>
-      <c r="M37" s="9"/>
-      <c r="N37" s="9"/>
-      <c r="O37" s="20"/>
+      <c r="M37" s="59"/>
+      <c r="N37" s="59"/>
+      <c r="O37" s="60"/>
     </row>
     <row r="38" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="B38" s="9" t="s">
+      <c r="A38" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="C38" s="20"/>
-      <c r="D38" s="38"/>
-      <c r="E38" s="39"/>
-      <c r="F38" s="39"/>
-      <c r="G38" s="39"/>
-      <c r="H38" s="39"/>
-      <c r="I38" s="39"/>
-      <c r="J38" s="40"/>
-      <c r="K38" s="29" t="s">
-        <v>54</v>
-      </c>
-      <c r="L38" s="9" t="s">
+      <c r="C38" s="60"/>
+      <c r="D38" s="68"/>
+      <c r="E38" s="69"/>
+      <c r="F38" s="69"/>
+      <c r="G38" s="69"/>
+      <c r="H38" s="69"/>
+      <c r="I38" s="69"/>
+      <c r="J38" s="70"/>
+      <c r="K38" s="65" t="s">
+        <v>54</v>
+      </c>
+      <c r="L38" s="59" t="s">
         <v>110</v>
       </c>
-      <c r="M38" s="9"/>
-      <c r="N38" s="9"/>
-      <c r="O38" s="20"/>
+      <c r="M38" s="59"/>
+      <c r="N38" s="59"/>
+      <c r="O38" s="60"/>
     </row>
     <row r="39" spans="1:15" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="B39" s="9" t="s">
+      <c r="A39" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="B39" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="C39" s="20"/>
-      <c r="D39" s="36"/>
-      <c r="E39" s="41"/>
-      <c r="F39" s="41"/>
-      <c r="G39" s="41"/>
-      <c r="H39" s="41"/>
-      <c r="I39" s="41"/>
-      <c r="J39" s="37"/>
-      <c r="K39" s="30" t="s">
-        <v>54</v>
-      </c>
-      <c r="L39" s="21" t="s">
+      <c r="C39" s="60"/>
+      <c r="D39" s="25"/>
+      <c r="E39" s="36"/>
+      <c r="F39" s="36"/>
+      <c r="G39" s="36"/>
+      <c r="H39" s="36"/>
+      <c r="I39" s="36"/>
+      <c r="J39" s="26"/>
+      <c r="K39" s="67" t="s">
+        <v>54</v>
+      </c>
+      <c r="L39" s="62" t="s">
         <v>105</v>
       </c>
-      <c r="M39" s="21"/>
-      <c r="N39" s="21"/>
-      <c r="O39" s="22"/>
+      <c r="M39" s="62"/>
+      <c r="N39" s="62"/>
+      <c r="O39" s="63"/>
     </row>
     <row r="40" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="B40" s="9" t="s">
+      <c r="A40" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="B40" s="59" t="s">
         <v>30</v>
       </c>
-      <c r="C40" s="20"/>
-      <c r="D40" s="43" t="s">
+      <c r="C40" s="60"/>
+      <c r="D40" s="72" t="s">
         <v>127</v>
       </c>
-      <c r="E40" s="44"/>
-      <c r="F40" s="44"/>
-      <c r="G40" s="44"/>
-      <c r="H40" s="44"/>
-      <c r="I40" s="44"/>
-      <c r="J40" s="44"/>
-      <c r="K40" s="44"/>
-      <c r="L40" s="44"/>
-      <c r="M40" s="44"/>
-      <c r="N40" s="44"/>
-      <c r="O40" s="45"/>
+      <c r="E40" s="73"/>
+      <c r="F40" s="73"/>
+      <c r="G40" s="73"/>
+      <c r="H40" s="73"/>
+      <c r="I40" s="73"/>
+      <c r="J40" s="73"/>
+      <c r="K40" s="73"/>
+      <c r="L40" s="73"/>
+      <c r="M40" s="73"/>
+      <c r="N40" s="73"/>
+      <c r="O40" s="74"/>
     </row>
     <row r="41" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="B41" s="9" t="s">
+      <c r="A41" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="B41" s="59" t="s">
         <v>31</v>
       </c>
-      <c r="C41" s="20"/>
-      <c r="D41" s="46"/>
-      <c r="E41" s="47"/>
-      <c r="F41" s="47"/>
-      <c r="G41" s="47"/>
-      <c r="H41" s="47"/>
-      <c r="I41" s="47"/>
-      <c r="J41" s="47"/>
-      <c r="K41" s="47"/>
-      <c r="L41" s="47"/>
-      <c r="M41" s="47"/>
-      <c r="N41" s="47"/>
-      <c r="O41" s="48"/>
+      <c r="C41" s="60"/>
+      <c r="D41" s="75"/>
+      <c r="E41" s="76"/>
+      <c r="F41" s="76"/>
+      <c r="G41" s="76"/>
+      <c r="H41" s="76"/>
+      <c r="I41" s="76"/>
+      <c r="J41" s="76"/>
+      <c r="K41" s="76"/>
+      <c r="L41" s="76"/>
+      <c r="M41" s="76"/>
+      <c r="N41" s="76"/>
+      <c r="O41" s="77"/>
     </row>
     <row r="42" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="B42" s="9" t="s">
+      <c r="A42" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="B42" s="59" t="s">
         <v>32</v>
       </c>
-      <c r="C42" s="20"/>
-      <c r="D42" s="38"/>
-      <c r="E42" s="39"/>
-      <c r="F42" s="39"/>
-      <c r="G42" s="39"/>
-      <c r="H42" s="39"/>
-      <c r="I42" s="39"/>
-      <c r="J42" s="39"/>
-      <c r="K42" s="39"/>
-      <c r="L42" s="39"/>
-      <c r="M42" s="39"/>
-      <c r="N42" s="39"/>
-      <c r="O42" s="40"/>
+      <c r="C42" s="60"/>
+      <c r="D42" s="68"/>
+      <c r="E42" s="69"/>
+      <c r="F42" s="69"/>
+      <c r="G42" s="69"/>
+      <c r="H42" s="69"/>
+      <c r="I42" s="69"/>
+      <c r="J42" s="69"/>
+      <c r="K42" s="69"/>
+      <c r="L42" s="69"/>
+      <c r="M42" s="69"/>
+      <c r="N42" s="69"/>
+      <c r="O42" s="70"/>
     </row>
     <row r="43" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="B43" s="9" t="s">
+      <c r="A43" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="B43" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="C43" s="20"/>
-      <c r="D43" s="38"/>
-      <c r="E43" s="39"/>
-      <c r="F43" s="39"/>
-      <c r="G43" s="39"/>
-      <c r="H43" s="39"/>
-      <c r="I43" s="39"/>
-      <c r="J43" s="39"/>
-      <c r="K43" s="39"/>
-      <c r="L43" s="39"/>
-      <c r="M43" s="39"/>
-      <c r="N43" s="39"/>
-      <c r="O43" s="40"/>
+      <c r="C43" s="60"/>
+      <c r="D43" s="68"/>
+      <c r="E43" s="69"/>
+      <c r="F43" s="69"/>
+      <c r="G43" s="69"/>
+      <c r="H43" s="69"/>
+      <c r="I43" s="69"/>
+      <c r="J43" s="69"/>
+      <c r="K43" s="69"/>
+      <c r="L43" s="69"/>
+      <c r="M43" s="69"/>
+      <c r="N43" s="69"/>
+      <c r="O43" s="70"/>
     </row>
     <row r="44" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="B44" s="9" t="s">
+      <c r="A44" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="B44" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="C44" s="20"/>
-      <c r="D44" s="38"/>
-      <c r="E44" s="39"/>
-      <c r="F44" s="39"/>
-      <c r="G44" s="39"/>
-      <c r="H44" s="39"/>
-      <c r="I44" s="39"/>
-      <c r="J44" s="39"/>
-      <c r="K44" s="39"/>
-      <c r="L44" s="39"/>
-      <c r="M44" s="39"/>
-      <c r="N44" s="39"/>
-      <c r="O44" s="40"/>
+      <c r="C44" s="60"/>
+      <c r="D44" s="68"/>
+      <c r="E44" s="69"/>
+      <c r="F44" s="69"/>
+      <c r="G44" s="69"/>
+      <c r="H44" s="69"/>
+      <c r="I44" s="69"/>
+      <c r="J44" s="69"/>
+      <c r="K44" s="69"/>
+      <c r="L44" s="69"/>
+      <c r="M44" s="69"/>
+      <c r="N44" s="69"/>
+      <c r="O44" s="70"/>
     </row>
     <row r="45" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="B45" s="9" t="s">
+      <c r="A45" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="B45" s="59" t="s">
         <v>35</v>
       </c>
-      <c r="C45" s="20"/>
-      <c r="D45" s="38"/>
-      <c r="E45" s="39"/>
-      <c r="F45" s="39"/>
-      <c r="G45" s="39"/>
-      <c r="H45" s="39"/>
-      <c r="I45" s="39"/>
-      <c r="J45" s="39"/>
-      <c r="K45" s="39"/>
-      <c r="L45" s="39"/>
-      <c r="M45" s="39"/>
-      <c r="N45" s="39"/>
-      <c r="O45" s="40"/>
+      <c r="C45" s="60"/>
+      <c r="D45" s="68"/>
+      <c r="E45" s="69"/>
+      <c r="F45" s="69"/>
+      <c r="G45" s="69"/>
+      <c r="H45" s="69"/>
+      <c r="I45" s="69"/>
+      <c r="J45" s="69"/>
+      <c r="K45" s="69"/>
+      <c r="L45" s="69"/>
+      <c r="M45" s="69"/>
+      <c r="N45" s="69"/>
+      <c r="O45" s="70"/>
     </row>
     <row r="46" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="B46" s="9" t="s">
+      <c r="A46" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="B46" s="59" t="s">
         <v>36</v>
       </c>
-      <c r="C46" s="20"/>
-      <c r="D46" s="38"/>
-      <c r="E46" s="39"/>
-      <c r="F46" s="39"/>
-      <c r="G46" s="39"/>
-      <c r="H46" s="39"/>
-      <c r="I46" s="39"/>
-      <c r="J46" s="39"/>
-      <c r="K46" s="39"/>
-      <c r="L46" s="39"/>
-      <c r="M46" s="39"/>
-      <c r="N46" s="39"/>
-      <c r="O46" s="40"/>
+      <c r="C46" s="60"/>
+      <c r="D46" s="68"/>
+      <c r="E46" s="69"/>
+      <c r="F46" s="69"/>
+      <c r="G46" s="69"/>
+      <c r="H46" s="69"/>
+      <c r="I46" s="69"/>
+      <c r="J46" s="69"/>
+      <c r="K46" s="69"/>
+      <c r="L46" s="69"/>
+      <c r="M46" s="69"/>
+      <c r="N46" s="69"/>
+      <c r="O46" s="70"/>
     </row>
     <row r="47" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="27" t="s">
-        <v>54</v>
-      </c>
-      <c r="B47" s="9" t="s">
+      <c r="A47" s="61" t="s">
+        <v>54</v>
+      </c>
+      <c r="B47" s="59" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="20"/>
-      <c r="D47" s="38"/>
-      <c r="E47" s="39"/>
-      <c r="F47" s="39"/>
-      <c r="G47" s="39"/>
-      <c r="H47" s="39"/>
-      <c r="I47" s="39"/>
-      <c r="J47" s="39"/>
-      <c r="K47" s="39"/>
-      <c r="L47" s="39"/>
-      <c r="M47" s="39"/>
-      <c r="N47" s="39"/>
-      <c r="O47" s="40"/>
+      <c r="C47" s="60"/>
+      <c r="D47" s="68"/>
+      <c r="E47" s="69"/>
+      <c r="F47" s="69"/>
+      <c r="G47" s="69"/>
+      <c r="H47" s="69"/>
+      <c r="I47" s="69"/>
+      <c r="J47" s="69"/>
+      <c r="K47" s="69"/>
+      <c r="L47" s="69"/>
+      <c r="M47" s="69"/>
+      <c r="N47" s="69"/>
+      <c r="O47" s="70"/>
     </row>
     <row r="48" spans="1:15" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="28" t="s">
-        <v>54</v>
-      </c>
-      <c r="B48" s="21" t="s">
+      <c r="A48" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="B48" s="62" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="22"/>
-      <c r="D48" s="36"/>
-      <c r="E48" s="41"/>
-      <c r="F48" s="41"/>
-      <c r="G48" s="41"/>
-      <c r="H48" s="41"/>
-      <c r="I48" s="41"/>
-      <c r="J48" s="41"/>
-      <c r="K48" s="41"/>
-      <c r="L48" s="41"/>
-      <c r="M48" s="41"/>
-      <c r="N48" s="41"/>
-      <c r="O48" s="37"/>
+      <c r="C48" s="63"/>
+      <c r="D48" s="25"/>
+      <c r="E48" s="36"/>
+      <c r="F48" s="36"/>
+      <c r="G48" s="36"/>
+      <c r="H48" s="36"/>
+      <c r="I48" s="36"/>
+      <c r="J48" s="36"/>
+      <c r="K48" s="36"/>
+      <c r="L48" s="36"/>
+      <c r="M48" s="36"/>
+      <c r="N48" s="36"/>
+      <c r="O48" s="26"/>
     </row>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="N26:O27"/>
+    <mergeCell ref="N25:O25"/>
+    <mergeCell ref="L4:M4"/>
+    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="L6:O7"/>
+    <mergeCell ref="D37:J39"/>
+    <mergeCell ref="D40:O41"/>
+    <mergeCell ref="D42:O48"/>
+    <mergeCell ref="A9:C9"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="H9:J9"/>
+    <mergeCell ref="K9:O9"/>
+    <mergeCell ref="D31:J31"/>
+    <mergeCell ref="D36:J36"/>
+    <mergeCell ref="D32:J35"/>
+    <mergeCell ref="K34:O34"/>
+    <mergeCell ref="K31:O31"/>
+    <mergeCell ref="K25:M25"/>
+    <mergeCell ref="K29:O30"/>
+    <mergeCell ref="K26:M27"/>
+    <mergeCell ref="K28:O28"/>
     <mergeCell ref="B2:I2"/>
     <mergeCell ref="K2:O2"/>
     <mergeCell ref="C3:F3"/>
@@ -2376,29 +2451,8 @@
     <mergeCell ref="G4:I4"/>
     <mergeCell ref="B6:E6"/>
     <mergeCell ref="J6:K7"/>
-    <mergeCell ref="D37:J39"/>
-    <mergeCell ref="D40:O41"/>
-    <mergeCell ref="D42:O48"/>
-    <mergeCell ref="A9:C9"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="H9:J9"/>
-    <mergeCell ref="K9:O9"/>
-    <mergeCell ref="D31:J31"/>
-    <mergeCell ref="D36:J36"/>
-    <mergeCell ref="D32:J35"/>
-    <mergeCell ref="K34:O34"/>
-    <mergeCell ref="K31:O31"/>
-    <mergeCell ref="K25:M25"/>
     <mergeCell ref="N3:O3"/>
     <mergeCell ref="N4:O4"/>
-    <mergeCell ref="K29:O30"/>
-    <mergeCell ref="K26:M27"/>
-    <mergeCell ref="K28:O28"/>
-    <mergeCell ref="N26:O27"/>
-    <mergeCell ref="N25:O25"/>
-    <mergeCell ref="L4:M4"/>
-    <mergeCell ref="L3:M3"/>
-    <mergeCell ref="L6:O7"/>
   </mergeCells>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
   <pageMargins left="3.9370078740157488E-3" right="0" top="0" bottom="0" header="0" footer="0"/>

</xml_diff>

<commit_message>
update framework n sich
</commit_message>
<xml_diff>
--- a/Docs/Excel/HB WO Form.xlsx
+++ b/Docs/Excel/HB WO Form.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="27045" windowHeight="16155" tabRatio="711"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27045" windowHeight="16155" tabRatio="711"/>
   </bookViews>
   <sheets>
     <sheet name="FORM" sheetId="11" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="522" uniqueCount="141">
   <si>
     <t>MECHANICAL FIRST WORD:</t>
   </si>
@@ -457,6 +457,24 @@
   </si>
   <si>
     <t>CAUSE CODE:</t>
+  </si>
+  <si>
+    <t>WORK ORDER NUMBER:</t>
+  </si>
+  <si>
+    <t>PM#</t>
+  </si>
+  <si>
+    <t>MECHANIC/E-TECH</t>
+  </si>
+  <si>
+    <t>P-TECH</t>
+  </si>
+  <si>
+    <t>M-TECH</t>
+  </si>
+  <si>
+    <t>First Word P-Tech</t>
   </si>
 </sst>
 </file>
@@ -522,12 +540,54 @@
       <name val="Roboto Condensed"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="mediumGray">
+        <fgColor theme="5" tint="0.59996337778862885"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="11">
@@ -646,7 +706,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="131">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -679,185 +739,362 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1142,10 +1379,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O48"/>
+  <dimension ref="A1:U48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:C9"/>
+      <selection activeCell="T34" sqref="T34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.3"/>
@@ -1161,1208 +1398,1303 @@
     <col min="13" max="13" width="10.625" style="8" customWidth="1"/>
     <col min="14" max="14" width="6.5" style="8" customWidth="1"/>
     <col min="15" max="15" width="7.875" style="8" customWidth="1"/>
-    <col min="16" max="16384" width="9" style="8"/>
+    <col min="16" max="16" width="9" style="8"/>
+    <col min="17" max="17" width="23.625" style="18" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:15" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="1:20" ht="39" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11"/>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="20" t="s">
         <v>92</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
-      <c r="H2" s="12"/>
-      <c r="I2" s="12"/>
-      <c r="J2" s="13" t="s">
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="20"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="108" t="s">
         <v>99</v>
       </c>
-      <c r="K2" s="14"/>
-      <c r="L2" s="14"/>
-      <c r="M2" s="14"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="16"/>
-    </row>
-    <row r="3" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="17"/>
-      <c r="B3" s="18" t="s">
+      <c r="K2" s="109"/>
+      <c r="L2" s="109"/>
+      <c r="M2" s="109"/>
+      <c r="N2" s="94"/>
+      <c r="O2" s="95"/>
+    </row>
+    <row r="3" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="115"/>
+      <c r="B3" s="116" t="s">
         <v>93</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="112" t="s">
         <v>94</v>
       </c>
-      <c r="D3" s="20"/>
-      <c r="E3" s="20"/>
-      <c r="F3" s="21"/>
-      <c r="G3" s="19" t="s">
+      <c r="D3" s="113"/>
+      <c r="E3" s="113"/>
+      <c r="F3" s="114"/>
+      <c r="G3" s="112" t="s">
         <v>95</v>
       </c>
-      <c r="H3" s="20"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="22" t="s">
+      <c r="H3" s="113"/>
+      <c r="I3" s="114"/>
+      <c r="J3" s="110" t="s">
         <v>96</v>
       </c>
-      <c r="K3" s="23"/>
-      <c r="L3" s="19" t="s">
+      <c r="K3" s="111"/>
+      <c r="L3" s="112" t="s">
         <v>97</v>
       </c>
-      <c r="M3" s="20"/>
-      <c r="N3" s="19" t="s">
+      <c r="M3" s="113"/>
+      <c r="N3" s="112" t="s">
         <v>98</v>
       </c>
-      <c r="O3" s="21"/>
-    </row>
-    <row r="4" spans="1:15" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="24"/>
-      <c r="B4" s="25"/>
-      <c r="C4" s="24"/>
-      <c r="D4" s="26"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="24"/>
-      <c r="H4" s="26"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="24"/>
-      <c r="K4" s="25"/>
-      <c r="L4" s="24"/>
-      <c r="M4" s="26"/>
-      <c r="N4" s="24"/>
-      <c r="O4" s="25"/>
-    </row>
-    <row r="5" spans="1:15" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="27"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
-      <c r="F5" s="27"/>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27"/>
-      <c r="I5" s="27"/>
-      <c r="J5" s="27"/>
-      <c r="K5" s="27"/>
-      <c r="L5" s="27"/>
-      <c r="M5" s="27"/>
-      <c r="N5" s="27"/>
-      <c r="O5" s="28"/>
-    </row>
-    <row r="6" spans="1:15" s="10" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="29"/>
-      <c r="B6" s="30" t="s">
+      <c r="O3" s="114"/>
+    </row>
+    <row r="4" spans="1:20" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="99"/>
+      <c r="B4" s="101"/>
+      <c r="C4" s="99"/>
+      <c r="D4" s="100"/>
+      <c r="E4" s="100"/>
+      <c r="F4" s="101"/>
+      <c r="G4" s="99"/>
+      <c r="H4" s="100"/>
+      <c r="I4" s="101"/>
+      <c r="J4" s="99"/>
+      <c r="K4" s="101"/>
+      <c r="L4" s="99"/>
+      <c r="M4" s="100"/>
+      <c r="N4" s="99"/>
+      <c r="O4" s="101"/>
+    </row>
+    <row r="5" spans="1:20" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="12"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="12"/>
+      <c r="O5" s="13"/>
+    </row>
+    <row r="6" spans="1:20" s="10" customFormat="1" ht="26.25" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="117"/>
+      <c r="B6" s="118" t="s">
         <v>82</v>
       </c>
-      <c r="C6" s="30"/>
-      <c r="D6" s="30"/>
-      <c r="E6" s="31"/>
-      <c r="F6" s="32" t="s">
-        <v>54</v>
-      </c>
-      <c r="G6" s="15" t="s">
+      <c r="C6" s="118"/>
+      <c r="D6" s="118"/>
+      <c r="E6" s="119"/>
+      <c r="F6" s="31" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="H6" s="15"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="33" t="s">
+      <c r="H6" s="22"/>
+      <c r="I6" s="23"/>
+      <c r="J6" s="123" t="s">
         <v>126</v>
       </c>
-      <c r="K6" s="34"/>
-      <c r="L6" s="35"/>
-      <c r="M6" s="35"/>
-      <c r="N6" s="35"/>
-      <c r="O6" s="36"/>
-    </row>
-    <row r="7" spans="1:15" s="10" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="37"/>
-      <c r="B7" s="38"/>
-      <c r="C7" s="38"/>
-      <c r="D7" s="38"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="40" t="s">
-        <v>54</v>
-      </c>
-      <c r="G7" s="41" t="s">
+      <c r="K6" s="124"/>
+      <c r="L6" s="125"/>
+      <c r="M6" s="125"/>
+      <c r="N6" s="125"/>
+      <c r="O6" s="126"/>
+      <c r="Q6" s="19"/>
+    </row>
+    <row r="7" spans="1:20" s="10" customFormat="1" ht="26.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="120"/>
+      <c r="B7" s="121"/>
+      <c r="C7" s="121"/>
+      <c r="D7" s="121"/>
+      <c r="E7" s="122"/>
+      <c r="F7" s="67" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" s="68" t="s">
         <v>86</v>
       </c>
-      <c r="H7" s="41"/>
-      <c r="I7" s="42"/>
-      <c r="J7" s="43"/>
-      <c r="K7" s="44"/>
-      <c r="L7" s="45"/>
-      <c r="M7" s="45"/>
-      <c r="N7" s="45"/>
-      <c r="O7" s="46"/>
-    </row>
-    <row r="8" spans="1:15" s="10" customFormat="1" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="47"/>
-      <c r="B8" s="47"/>
-      <c r="C8" s="47"/>
-      <c r="D8" s="47"/>
-      <c r="E8" s="47"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="48"/>
-      <c r="H8" s="49"/>
-      <c r="I8" s="49"/>
-      <c r="J8" s="27"/>
-      <c r="K8" s="50"/>
-      <c r="L8" s="50"/>
-      <c r="M8" s="50"/>
-      <c r="N8" s="50"/>
-      <c r="O8" s="50"/>
-    </row>
-    <row r="9" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="51" t="s">
+      <c r="H7" s="68"/>
+      <c r="I7" s="69"/>
+      <c r="J7" s="127"/>
+      <c r="K7" s="128"/>
+      <c r="L7" s="129"/>
+      <c r="M7" s="129"/>
+      <c r="N7" s="129"/>
+      <c r="O7" s="130"/>
+      <c r="Q7" s="19"/>
+    </row>
+    <row r="8" spans="1:20" s="10" customFormat="1" ht="3.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
+      <c r="E8" s="14"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="16"/>
+      <c r="I8" s="16"/>
+      <c r="J8" s="12"/>
+      <c r="K8" s="17"/>
+      <c r="L8" s="17"/>
+      <c r="M8" s="17"/>
+      <c r="N8" s="17"/>
+      <c r="O8" s="17"/>
+      <c r="Q8" s="19"/>
+    </row>
+    <row r="9" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="21" t="s">
         <v>128</v>
       </c>
-      <c r="B9" s="15"/>
-      <c r="C9" s="16"/>
-      <c r="D9" s="51" t="s">
+      <c r="B9" s="22"/>
+      <c r="C9" s="23"/>
+      <c r="D9" s="70" t="s">
         <v>130</v>
       </c>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="52"/>
-      <c r="H9" s="51" t="s">
+      <c r="E9" s="71"/>
+      <c r="F9" s="71"/>
+      <c r="G9" s="72"/>
+      <c r="H9" s="81" t="s">
         <v>129</v>
       </c>
-      <c r="I9" s="15"/>
-      <c r="J9" s="16"/>
-      <c r="K9" s="51" t="s">
+      <c r="I9" s="82"/>
+      <c r="J9" s="83"/>
+      <c r="K9" s="32" t="s">
         <v>131</v>
       </c>
-      <c r="L9" s="15"/>
-      <c r="M9" s="15"/>
-      <c r="N9" s="15"/>
-      <c r="O9" s="16"/>
-    </row>
-    <row r="10" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="53"/>
-      <c r="B10" s="28" t="s">
+      <c r="L9" s="33"/>
+      <c r="M9" s="33"/>
+      <c r="N9" s="33"/>
+      <c r="O9" s="34"/>
+    </row>
+    <row r="10" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="24"/>
+      <c r="B10" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="54"/>
-      <c r="D10" s="55"/>
-      <c r="E10" s="28" t="s">
+      <c r="C10" s="26"/>
+      <c r="D10" s="73"/>
+      <c r="E10" s="74" t="s">
         <v>1</v>
       </c>
-      <c r="F10" s="28"/>
-      <c r="G10" s="54"/>
-      <c r="H10" s="55"/>
-      <c r="I10" s="28" t="s">
+      <c r="F10" s="74"/>
+      <c r="G10" s="75"/>
+      <c r="H10" s="84"/>
+      <c r="I10" s="85" t="s">
         <v>1</v>
       </c>
-      <c r="J10" s="54"/>
-      <c r="K10" s="55"/>
-      <c r="L10" s="28" t="s">
+      <c r="J10" s="86"/>
+      <c r="K10" s="35"/>
+      <c r="L10" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="M10" s="28"/>
-      <c r="N10" s="28"/>
-      <c r="O10" s="54"/>
-    </row>
-    <row r="11" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="B11" s="28" t="s">
+      <c r="M10" s="36"/>
+      <c r="N10" s="36"/>
+      <c r="O10" s="37"/>
+      <c r="Q10" s="18" t="s">
+        <v>135</v>
+      </c>
+      <c r="T10" s="65" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C11" s="54"/>
-      <c r="D11" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="E11" s="28" t="s">
+      <c r="C11" s="26"/>
+      <c r="D11" s="76" t="s">
+        <v>54</v>
+      </c>
+      <c r="E11" s="74" t="s">
         <v>112</v>
       </c>
-      <c r="F11" s="28"/>
-      <c r="G11" s="54"/>
-      <c r="H11" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="I11" s="28" t="s">
+      <c r="F11" s="74"/>
+      <c r="G11" s="75"/>
+      <c r="H11" s="87" t="s">
+        <v>54</v>
+      </c>
+      <c r="I11" s="85" t="s">
         <v>56</v>
       </c>
-      <c r="J11" s="54"/>
-      <c r="K11" s="57" t="s">
-        <v>54</v>
-      </c>
-      <c r="L11" s="28" t="s">
+      <c r="J11" s="86"/>
+      <c r="K11" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="L11" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="M11" s="28"/>
-      <c r="N11" s="28"/>
-      <c r="O11" s="54"/>
-    </row>
-    <row r="12" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="B12" s="28" t="s">
+      <c r="M11" s="36"/>
+      <c r="N11" s="36"/>
+      <c r="O11" s="37"/>
+      <c r="Q11" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="T11" s="66" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B12" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="C12" s="54"/>
-      <c r="D12" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="E12" s="28" t="s">
+      <c r="C12" s="26"/>
+      <c r="D12" s="76" t="s">
+        <v>54</v>
+      </c>
+      <c r="E12" s="74" t="s">
         <v>113</v>
       </c>
-      <c r="F12" s="28"/>
-      <c r="G12" s="54"/>
-      <c r="H12" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="I12" s="28" t="s">
+      <c r="F12" s="74"/>
+      <c r="G12" s="75"/>
+      <c r="H12" s="87" t="s">
+        <v>54</v>
+      </c>
+      <c r="I12" s="85" t="s">
         <v>57</v>
       </c>
-      <c r="J12" s="54"/>
-      <c r="K12" s="57" t="s">
-        <v>54</v>
-      </c>
-      <c r="L12" s="28" t="s">
+      <c r="J12" s="86"/>
+      <c r="K12" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="L12" s="36" t="s">
         <v>50</v>
       </c>
-      <c r="M12" s="28"/>
-      <c r="N12" s="28"/>
-      <c r="O12" s="54"/>
-    </row>
-    <row r="13" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="B13" s="28" t="s">
+      <c r="M12" s="36"/>
+      <c r="N12" s="36"/>
+      <c r="O12" s="37"/>
+      <c r="Q12" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="T12" s="80" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B13" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="C13" s="54"/>
-      <c r="D13" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="E13" s="28" t="s">
+      <c r="C13" s="26"/>
+      <c r="D13" s="76" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="74" t="s">
         <v>114</v>
       </c>
-      <c r="F13" s="28"/>
-      <c r="G13" s="54"/>
-      <c r="H13" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="I13" s="28" t="s">
+      <c r="F13" s="74"/>
+      <c r="G13" s="75"/>
+      <c r="H13" s="87" t="s">
+        <v>54</v>
+      </c>
+      <c r="I13" s="85" t="s">
         <v>58</v>
       </c>
-      <c r="J13" s="54"/>
-      <c r="K13" s="57" t="s">
-        <v>54</v>
-      </c>
-      <c r="L13" s="28" t="s">
+      <c r="J13" s="86"/>
+      <c r="K13" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="L13" s="36" t="s">
         <v>51</v>
       </c>
-      <c r="M13" s="28"/>
-      <c r="N13" s="28"/>
-      <c r="O13" s="54"/>
-    </row>
-    <row r="14" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="B14" s="28" t="s">
+      <c r="M13" s="36"/>
+      <c r="N13" s="36"/>
+      <c r="O13" s="37"/>
+      <c r="Q13" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B14" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="54"/>
-      <c r="D14" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="E14" s="28" t="s">
+      <c r="C14" s="26"/>
+      <c r="D14" s="76" t="s">
+        <v>54</v>
+      </c>
+      <c r="E14" s="74" t="s">
         <v>115</v>
       </c>
-      <c r="F14" s="28"/>
-      <c r="G14" s="54"/>
-      <c r="H14" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="I14" s="28" t="s">
+      <c r="F14" s="74"/>
+      <c r="G14" s="75"/>
+      <c r="H14" s="87" t="s">
+        <v>54</v>
+      </c>
+      <c r="I14" s="85" t="s">
         <v>59</v>
       </c>
-      <c r="J14" s="54"/>
-      <c r="K14" s="57" t="s">
-        <v>54</v>
-      </c>
-      <c r="L14" s="28" t="s">
+      <c r="J14" s="86"/>
+      <c r="K14" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="L14" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="M14" s="28"/>
-      <c r="N14" s="28"/>
-      <c r="O14" s="54"/>
-    </row>
-    <row r="15" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="B15" s="28" t="s">
+      <c r="M14" s="36"/>
+      <c r="N14" s="36"/>
+      <c r="O14" s="37"/>
+      <c r="Q14" s="18" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="C15" s="54"/>
-      <c r="D15" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="E15" s="28" t="s">
+      <c r="C15" s="26"/>
+      <c r="D15" s="76" t="s">
+        <v>54</v>
+      </c>
+      <c r="E15" s="74" t="s">
         <v>116</v>
       </c>
-      <c r="F15" s="28"/>
-      <c r="G15" s="54"/>
-      <c r="H15" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="I15" s="28" t="s">
+      <c r="F15" s="74"/>
+      <c r="G15" s="75"/>
+      <c r="H15" s="87" t="s">
+        <v>54</v>
+      </c>
+      <c r="I15" s="85" t="s">
         <v>60</v>
       </c>
-      <c r="J15" s="54"/>
-      <c r="K15" s="57" t="s">
-        <v>54</v>
-      </c>
-      <c r="L15" s="28" t="s">
+      <c r="J15" s="86"/>
+      <c r="K15" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="L15" s="36" t="s">
         <v>53</v>
       </c>
-      <c r="M15" s="28"/>
-      <c r="N15" s="28"/>
-      <c r="O15" s="54"/>
-    </row>
-    <row r="16" spans="1:15" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="B16" s="28" t="s">
+      <c r="M15" s="36"/>
+      <c r="N15" s="36"/>
+      <c r="O15" s="37"/>
+      <c r="Q15" s="18" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B16" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="54"/>
-      <c r="D16" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="E16" s="28" t="s">
+      <c r="C16" s="26"/>
+      <c r="D16" s="76" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" s="74" t="s">
         <v>117</v>
       </c>
-      <c r="F16" s="28"/>
-      <c r="G16" s="54"/>
-      <c r="H16" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="I16" s="28" t="s">
+      <c r="F16" s="74"/>
+      <c r="G16" s="75"/>
+      <c r="H16" s="87" t="s">
+        <v>54</v>
+      </c>
+      <c r="I16" s="85" t="s">
         <v>61</v>
       </c>
-      <c r="J16" s="54"/>
-      <c r="K16" s="55"/>
-      <c r="L16" s="28" t="s">
+      <c r="J16" s="86"/>
+      <c r="K16" s="35"/>
+      <c r="L16" s="36" t="s">
         <v>125</v>
       </c>
-      <c r="M16" s="28"/>
-      <c r="N16" s="28"/>
-      <c r="O16" s="54"/>
-    </row>
-    <row r="17" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="B17" s="28" t="s">
+      <c r="M16" s="36"/>
+      <c r="N16" s="36"/>
+      <c r="O16" s="37"/>
+      <c r="Q16" s="18" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B17" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="54"/>
-      <c r="D17" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="E17" s="28" t="s">
+      <c r="C17" s="26"/>
+      <c r="D17" s="76" t="s">
+        <v>54</v>
+      </c>
+      <c r="E17" s="74" t="s">
         <v>118</v>
       </c>
-      <c r="F17" s="28"/>
-      <c r="G17" s="54"/>
-      <c r="H17" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="I17" s="28" t="s">
+      <c r="F17" s="74"/>
+      <c r="G17" s="75"/>
+      <c r="H17" s="87" t="s">
+        <v>54</v>
+      </c>
+      <c r="I17" s="85" t="s">
         <v>62</v>
       </c>
-      <c r="J17" s="28"/>
-      <c r="K17" s="17"/>
-      <c r="L17" s="58"/>
-      <c r="M17" s="58"/>
-      <c r="N17" s="58"/>
-      <c r="O17" s="18"/>
-    </row>
-    <row r="18" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="B18" s="28" t="s">
+      <c r="J17" s="85"/>
+      <c r="K17" s="39"/>
+      <c r="L17" s="40"/>
+      <c r="M17" s="40"/>
+      <c r="N17" s="40"/>
+      <c r="O17" s="41"/>
+      <c r="Q17" s="18" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="54"/>
-      <c r="D18" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="E18" s="28" t="s">
+      <c r="C18" s="26"/>
+      <c r="D18" s="76" t="s">
+        <v>54</v>
+      </c>
+      <c r="E18" s="74" t="s">
         <v>119</v>
       </c>
-      <c r="F18" s="28"/>
-      <c r="G18" s="54"/>
-      <c r="H18" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="I18" s="28" t="s">
+      <c r="F18" s="74"/>
+      <c r="G18" s="75"/>
+      <c r="H18" s="87" t="s">
+        <v>54</v>
+      </c>
+      <c r="I18" s="85" t="s">
         <v>63</v>
       </c>
-      <c r="J18" s="28"/>
-      <c r="K18" s="55"/>
-      <c r="L18" s="28" t="s">
+      <c r="J18" s="85"/>
+      <c r="K18" s="35"/>
+      <c r="L18" s="36" t="s">
         <v>75</v>
       </c>
-      <c r="M18" s="28"/>
-      <c r="N18" s="28"/>
-      <c r="O18" s="54"/>
-    </row>
-    <row r="19" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="B19" s="28" t="s">
+      <c r="M18" s="36"/>
+      <c r="N18" s="36"/>
+      <c r="O18" s="37"/>
+      <c r="Q18" s="18" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="C19" s="54"/>
-      <c r="D19" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="E19" s="28" t="s">
+      <c r="C19" s="26"/>
+      <c r="D19" s="76" t="s">
+        <v>54</v>
+      </c>
+      <c r="E19" s="74" t="s">
         <v>120</v>
       </c>
-      <c r="F19" s="28"/>
-      <c r="G19" s="54"/>
-      <c r="H19" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="I19" s="28" t="s">
+      <c r="F19" s="74"/>
+      <c r="G19" s="75"/>
+      <c r="H19" s="87" t="s">
+        <v>54</v>
+      </c>
+      <c r="I19" s="85" t="s">
         <v>64</v>
       </c>
-      <c r="J19" s="28"/>
-      <c r="K19" s="55"/>
-      <c r="L19" s="28" t="s">
+      <c r="J19" s="85"/>
+      <c r="K19" s="35"/>
+      <c r="L19" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="M19" s="28"/>
-      <c r="N19" s="28"/>
-      <c r="O19" s="54"/>
-    </row>
-    <row r="20" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="B20" s="28" t="s">
+      <c r="M19" s="36"/>
+      <c r="N19" s="36"/>
+      <c r="O19" s="37"/>
+      <c r="Q19" s="18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B20" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="C20" s="54"/>
-      <c r="D20" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="E20" s="28" t="s">
+      <c r="C20" s="26"/>
+      <c r="D20" s="76" t="s">
+        <v>54</v>
+      </c>
+      <c r="E20" s="74" t="s">
         <v>121</v>
       </c>
-      <c r="F20" s="28"/>
-      <c r="G20" s="54"/>
-      <c r="H20" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="I20" s="28" t="s">
+      <c r="F20" s="74"/>
+      <c r="G20" s="75"/>
+      <c r="H20" s="87" t="s">
+        <v>54</v>
+      </c>
+      <c r="I20" s="85" t="s">
         <v>65</v>
       </c>
-      <c r="J20" s="28"/>
-      <c r="K20" s="57" t="s">
-        <v>54</v>
-      </c>
-      <c r="L20" s="28" t="s">
+      <c r="J20" s="85"/>
+      <c r="K20" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="L20" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="M20" s="28"/>
-      <c r="N20" s="28"/>
-      <c r="O20" s="54"/>
-    </row>
-    <row r="21" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="B21" s="28" t="s">
+      <c r="M20" s="36"/>
+      <c r="N20" s="36"/>
+      <c r="O20" s="37"/>
+      <c r="Q20" s="18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B21" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="C21" s="54"/>
-      <c r="D21" s="55"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="28"/>
-      <c r="G21" s="54"/>
-      <c r="H21" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="I21" s="28" t="s">
+      <c r="C21" s="26"/>
+      <c r="D21" s="73"/>
+      <c r="E21" s="74"/>
+      <c r="F21" s="74"/>
+      <c r="G21" s="75"/>
+      <c r="H21" s="87" t="s">
+        <v>54</v>
+      </c>
+      <c r="I21" s="85" t="s">
         <v>66</v>
       </c>
-      <c r="J21" s="28"/>
-      <c r="K21" s="57" t="s">
-        <v>54</v>
-      </c>
-      <c r="L21" s="28" t="s">
+      <c r="J21" s="85"/>
+      <c r="K21" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="L21" s="36" t="s">
         <v>77</v>
       </c>
-      <c r="M21" s="28"/>
-      <c r="N21" s="28"/>
-      <c r="O21" s="54"/>
-    </row>
-    <row r="22" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="B22" s="28" t="s">
+      <c r="M21" s="36"/>
+      <c r="N21" s="36"/>
+      <c r="O21" s="37"/>
+      <c r="Q21" s="18" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B22" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="54"/>
-      <c r="D22" s="55"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-      <c r="G22" s="54"/>
-      <c r="H22" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="I22" s="28" t="s">
+      <c r="C22" s="26"/>
+      <c r="D22" s="73"/>
+      <c r="E22" s="74"/>
+      <c r="F22" s="74"/>
+      <c r="G22" s="75"/>
+      <c r="H22" s="87" t="s">
+        <v>54</v>
+      </c>
+      <c r="I22" s="85" t="s">
         <v>67</v>
       </c>
-      <c r="J22" s="28"/>
-      <c r="K22" s="57" t="s">
-        <v>54</v>
-      </c>
-      <c r="L22" s="28" t="s">
+      <c r="J22" s="85"/>
+      <c r="K22" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="L22" s="36" t="s">
         <v>78</v>
       </c>
-      <c r="M22" s="28"/>
-      <c r="N22" s="28"/>
-      <c r="O22" s="54"/>
-    </row>
-    <row r="23" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="B23" s="28" t="s">
+      <c r="M22" s="36"/>
+      <c r="N22" s="36"/>
+      <c r="O22" s="37"/>
+      <c r="Q22" s="18" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B23" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="C23" s="54"/>
-      <c r="D23" s="55"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
-      <c r="G23" s="54"/>
-      <c r="H23" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="I23" s="28" t="s">
+      <c r="C23" s="26"/>
+      <c r="D23" s="73"/>
+      <c r="E23" s="74"/>
+      <c r="F23" s="74"/>
+      <c r="G23" s="75"/>
+      <c r="H23" s="87" t="s">
+        <v>54</v>
+      </c>
+      <c r="I23" s="85" t="s">
         <v>68</v>
       </c>
-      <c r="J23" s="28"/>
-      <c r="K23" s="57" t="s">
-        <v>54</v>
-      </c>
-      <c r="L23" s="28" t="s">
+      <c r="J23" s="85"/>
+      <c r="K23" s="38" t="s">
+        <v>54</v>
+      </c>
+      <c r="L23" s="36" t="s">
         <v>79</v>
       </c>
-      <c r="M23" s="28"/>
-      <c r="N23" s="28"/>
-      <c r="O23" s="54"/>
-    </row>
-    <row r="24" spans="1:15" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="B24" s="28" t="s">
+      <c r="M23" s="36"/>
+      <c r="N23" s="36"/>
+      <c r="O23" s="37"/>
+      <c r="Q23" s="18" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B24" s="25" t="s">
         <v>15</v>
       </c>
-      <c r="C24" s="54"/>
-      <c r="D24" s="55"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
-      <c r="G24" s="54"/>
-      <c r="H24" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="I24" s="28" t="s">
+      <c r="C24" s="26"/>
+      <c r="D24" s="73"/>
+      <c r="E24" s="74"/>
+      <c r="F24" s="74"/>
+      <c r="G24" s="75"/>
+      <c r="H24" s="87" t="s">
+        <v>54</v>
+      </c>
+      <c r="I24" s="85" t="s">
         <v>69</v>
       </c>
-      <c r="J24" s="28"/>
-      <c r="K24" s="59" t="s">
-        <v>54</v>
-      </c>
-      <c r="L24" s="60" t="s">
+      <c r="J24" s="85"/>
+      <c r="K24" s="42" t="s">
+        <v>54</v>
+      </c>
+      <c r="L24" s="43" t="s">
         <v>80</v>
       </c>
-      <c r="M24" s="60"/>
-      <c r="N24" s="60"/>
-      <c r="O24" s="61"/>
-    </row>
-    <row r="25" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="B25" s="28" t="s">
+      <c r="M24" s="43"/>
+      <c r="N24" s="43"/>
+      <c r="O24" s="44"/>
+      <c r="Q24" s="18" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B25" s="25" t="s">
         <v>16</v>
       </c>
-      <c r="C25" s="54"/>
-      <c r="D25" s="55"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
-      <c r="G25" s="54"/>
-      <c r="H25" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="I25" s="28" t="s">
+      <c r="C25" s="26"/>
+      <c r="D25" s="73"/>
+      <c r="E25" s="74"/>
+      <c r="F25" s="74"/>
+      <c r="G25" s="75"/>
+      <c r="H25" s="87" t="s">
+        <v>54</v>
+      </c>
+      <c r="I25" s="85" t="s">
         <v>70</v>
       </c>
-      <c r="J25" s="28"/>
-      <c r="K25" s="19" t="s">
+      <c r="J25" s="85"/>
+      <c r="K25" s="45" t="s">
         <v>122</v>
       </c>
-      <c r="L25" s="20"/>
-      <c r="M25" s="21"/>
-      <c r="N25" s="19" t="s">
+      <c r="L25" s="46"/>
+      <c r="M25" s="47"/>
+      <c r="N25" s="45" t="s">
         <v>134</v>
       </c>
-      <c r="O25" s="21"/>
-    </row>
-    <row r="26" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="B26" s="28" t="s">
+      <c r="O25" s="47"/>
+      <c r="Q25" s="18" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="54"/>
-      <c r="D26" s="55"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="54"/>
-      <c r="H26" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="I26" s="28" t="s">
+      <c r="C26" s="26"/>
+      <c r="D26" s="73"/>
+      <c r="E26" s="74"/>
+      <c r="F26" s="74"/>
+      <c r="G26" s="75"/>
+      <c r="H26" s="87" t="s">
+        <v>54</v>
+      </c>
+      <c r="I26" s="85" t="s">
         <v>71</v>
       </c>
-      <c r="J26" s="28"/>
-      <c r="K26" s="62"/>
-      <c r="L26" s="63"/>
-      <c r="M26" s="64"/>
-      <c r="N26" s="62"/>
-      <c r="O26" s="64"/>
-    </row>
-    <row r="27" spans="1:15" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="B27" s="28" t="s">
+      <c r="J26" s="85"/>
+      <c r="K26" s="48"/>
+      <c r="L26" s="49"/>
+      <c r="M26" s="50"/>
+      <c r="N26" s="48"/>
+      <c r="O26" s="50"/>
+      <c r="Q26" s="18" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" s="25" t="s">
         <v>18</v>
       </c>
-      <c r="C27" s="54"/>
-      <c r="D27" s="55"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="54"/>
-      <c r="H27" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="I27" s="28" t="s">
+      <c r="C27" s="26"/>
+      <c r="D27" s="73"/>
+      <c r="E27" s="74"/>
+      <c r="F27" s="74"/>
+      <c r="G27" s="75"/>
+      <c r="H27" s="87" t="s">
+        <v>54</v>
+      </c>
+      <c r="I27" s="85" t="s">
         <v>72</v>
       </c>
-      <c r="J27" s="28"/>
-      <c r="K27" s="24"/>
-      <c r="L27" s="26"/>
-      <c r="M27" s="25"/>
-      <c r="N27" s="24"/>
-      <c r="O27" s="25"/>
-    </row>
-    <row r="28" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="B28" s="28" t="s">
+      <c r="J27" s="85"/>
+      <c r="K27" s="51"/>
+      <c r="L27" s="52"/>
+      <c r="M27" s="53"/>
+      <c r="N27" s="51"/>
+      <c r="O27" s="53"/>
+      <c r="Q27" s="18" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="C28" s="54"/>
-      <c r="D28" s="55"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-      <c r="G28" s="54"/>
-      <c r="H28" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="I28" s="28" t="s">
+      <c r="C28" s="26"/>
+      <c r="D28" s="73"/>
+      <c r="E28" s="74"/>
+      <c r="F28" s="74"/>
+      <c r="G28" s="75"/>
+      <c r="H28" s="87" t="s">
+        <v>54</v>
+      </c>
+      <c r="I28" s="85" t="s">
         <v>73</v>
       </c>
-      <c r="J28" s="28"/>
-      <c r="K28" s="19" t="s">
+      <c r="J28" s="85"/>
+      <c r="K28" s="45" t="s">
         <v>124</v>
       </c>
-      <c r="L28" s="20"/>
-      <c r="M28" s="20"/>
-      <c r="N28" s="20"/>
-      <c r="O28" s="21"/>
-    </row>
-    <row r="29" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="B29" s="28" t="s">
+      <c r="L28" s="46"/>
+      <c r="M28" s="46"/>
+      <c r="N28" s="46"/>
+      <c r="O28" s="47"/>
+      <c r="Q28" s="18" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="C29" s="54"/>
-      <c r="D29" s="55"/>
-      <c r="E29" s="28"/>
-      <c r="F29" s="28"/>
-      <c r="G29" s="54"/>
-      <c r="H29" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="I29" s="28" t="s">
+      <c r="C29" s="26"/>
+      <c r="D29" s="73"/>
+      <c r="E29" s="74"/>
+      <c r="F29" s="74"/>
+      <c r="G29" s="75"/>
+      <c r="H29" s="87" t="s">
+        <v>54</v>
+      </c>
+      <c r="I29" s="85" t="s">
         <v>74</v>
       </c>
-      <c r="J29" s="54"/>
-      <c r="K29" s="62"/>
-      <c r="L29" s="63"/>
-      <c r="M29" s="63"/>
-      <c r="N29" s="63"/>
-      <c r="O29" s="64"/>
-    </row>
-    <row r="30" spans="1:15" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="B30" s="28" t="s">
+      <c r="J29" s="86"/>
+      <c r="K29" s="48"/>
+      <c r="L29" s="49"/>
+      <c r="M29" s="49"/>
+      <c r="N29" s="49"/>
+      <c r="O29" s="50"/>
+      <c r="Q29" s="8" t="s">
+        <v>82</v>
+      </c>
+      <c r="T29" s="8" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A30" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B30" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="C30" s="54"/>
-      <c r="D30" s="65"/>
-      <c r="E30" s="60"/>
-      <c r="F30" s="60"/>
-      <c r="G30" s="61"/>
-      <c r="H30" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="I30" s="60" t="s">
+      <c r="C30" s="26"/>
+      <c r="D30" s="77"/>
+      <c r="E30" s="78"/>
+      <c r="F30" s="78"/>
+      <c r="G30" s="79"/>
+      <c r="H30" s="87" t="s">
+        <v>54</v>
+      </c>
+      <c r="I30" s="88" t="s">
         <v>37</v>
       </c>
-      <c r="J30" s="61"/>
-      <c r="K30" s="24"/>
-      <c r="L30" s="26"/>
-      <c r="M30" s="26"/>
-      <c r="N30" s="26"/>
-      <c r="O30" s="25"/>
-    </row>
-    <row r="31" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="B31" s="28" t="s">
+      <c r="J30" s="89"/>
+      <c r="K30" s="51"/>
+      <c r="L30" s="52"/>
+      <c r="M30" s="52"/>
+      <c r="N30" s="52"/>
+      <c r="O30" s="53"/>
+      <c r="Q30" s="8" t="s">
+        <v>137</v>
+      </c>
+      <c r="T30" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="U30" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="C31" s="54"/>
-      <c r="D31" s="51" t="s">
+    </row>
+    <row r="31" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B31" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="C31" s="26"/>
+      <c r="D31" s="93" t="s">
         <v>100</v>
       </c>
-      <c r="E31" s="15"/>
-      <c r="F31" s="15"/>
-      <c r="G31" s="15"/>
-      <c r="H31" s="15"/>
-      <c r="I31" s="15"/>
-      <c r="J31" s="16"/>
-      <c r="K31" s="51" t="s">
+      <c r="E31" s="94"/>
+      <c r="F31" s="94"/>
+      <c r="G31" s="94"/>
+      <c r="H31" s="94"/>
+      <c r="I31" s="94"/>
+      <c r="J31" s="95"/>
+      <c r="K31" s="54" t="s">
         <v>133</v>
       </c>
-      <c r="L31" s="15"/>
-      <c r="M31" s="15"/>
-      <c r="N31" s="15"/>
-      <c r="O31" s="16"/>
-    </row>
-    <row r="32" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="B32" s="28" t="s">
+      <c r="L31" s="55"/>
+      <c r="M31" s="55"/>
+      <c r="N31" s="55"/>
+      <c r="O31" s="56"/>
+      <c r="Q31" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="T31" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="U31" s="25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B32" s="25" t="s">
         <v>81</v>
       </c>
-      <c r="C32" s="54"/>
-      <c r="D32" s="62"/>
-      <c r="E32" s="63"/>
-      <c r="F32" s="63"/>
-      <c r="G32" s="63"/>
-      <c r="H32" s="63"/>
-      <c r="I32" s="63"/>
-      <c r="J32" s="64"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="96"/>
+      <c r="E32" s="97"/>
+      <c r="F32" s="97"/>
+      <c r="G32" s="97"/>
+      <c r="H32" s="97"/>
+      <c r="I32" s="97"/>
+      <c r="J32" s="98"/>
       <c r="K32" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="L32" s="28" t="s">
+      <c r="L32" s="58" t="s">
         <v>102</v>
       </c>
-      <c r="M32" s="28"/>
-      <c r="N32" s="28"/>
-      <c r="O32" s="54"/>
+      <c r="M32" s="58"/>
+      <c r="N32" s="58"/>
+      <c r="O32" s="59"/>
     </row>
     <row r="33" spans="1:15" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A33" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="B33" s="28" t="s">
+      <c r="A33" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B33" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="C33" s="54"/>
-      <c r="D33" s="62"/>
-      <c r="E33" s="63"/>
-      <c r="F33" s="63"/>
-      <c r="G33" s="63"/>
-      <c r="H33" s="63"/>
-      <c r="I33" s="63"/>
-      <c r="J33" s="64"/>
-      <c r="K33" s="65"/>
-      <c r="L33" s="60"/>
-      <c r="M33" s="60"/>
-      <c r="N33" s="60"/>
-      <c r="O33" s="61"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="96"/>
+      <c r="E33" s="97"/>
+      <c r="F33" s="97"/>
+      <c r="G33" s="97"/>
+      <c r="H33" s="97"/>
+      <c r="I33" s="97"/>
+      <c r="J33" s="98"/>
+      <c r="K33" s="60"/>
+      <c r="L33" s="61"/>
+      <c r="M33" s="61"/>
+      <c r="N33" s="61"/>
+      <c r="O33" s="62"/>
     </row>
     <row r="34" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="B34" s="28" t="s">
+      <c r="A34" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B34" s="25" t="s">
         <v>25</v>
       </c>
-      <c r="C34" s="54"/>
-      <c r="D34" s="62"/>
-      <c r="E34" s="63"/>
-      <c r="F34" s="63"/>
-      <c r="G34" s="63"/>
-      <c r="H34" s="63"/>
-      <c r="I34" s="63"/>
-      <c r="J34" s="64"/>
-      <c r="K34" s="51" t="s">
+      <c r="C34" s="26"/>
+      <c r="D34" s="96"/>
+      <c r="E34" s="97"/>
+      <c r="F34" s="97"/>
+      <c r="G34" s="97"/>
+      <c r="H34" s="97"/>
+      <c r="I34" s="97"/>
+      <c r="J34" s="98"/>
+      <c r="K34" s="54" t="s">
         <v>132</v>
       </c>
-      <c r="L34" s="15"/>
-      <c r="M34" s="15"/>
-      <c r="N34" s="15"/>
-      <c r="O34" s="16"/>
+      <c r="L34" s="55"/>
+      <c r="M34" s="55"/>
+      <c r="N34" s="55"/>
+      <c r="O34" s="56"/>
     </row>
     <row r="35" spans="1:15" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="B35" s="28" t="s">
+      <c r="A35" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B35" s="25" t="s">
         <v>26</v>
       </c>
-      <c r="C35" s="54"/>
-      <c r="D35" s="24"/>
-      <c r="E35" s="26"/>
-      <c r="F35" s="26"/>
-      <c r="G35" s="26"/>
-      <c r="H35" s="26"/>
-      <c r="I35" s="26"/>
-      <c r="J35" s="25"/>
-      <c r="K35" s="55"/>
-      <c r="L35" s="28" t="s">
+      <c r="C35" s="26"/>
+      <c r="D35" s="99"/>
+      <c r="E35" s="100"/>
+      <c r="F35" s="100"/>
+      <c r="G35" s="100"/>
+      <c r="H35" s="100"/>
+      <c r="I35" s="100"/>
+      <c r="J35" s="101"/>
+      <c r="K35" s="63"/>
+      <c r="L35" s="58" t="s">
         <v>1</v>
       </c>
-      <c r="M35" s="28"/>
-      <c r="N35" s="28"/>
-      <c r="O35" s="54"/>
+      <c r="M35" s="58"/>
+      <c r="N35" s="58"/>
+      <c r="O35" s="59"/>
     </row>
     <row r="36" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="B36" s="28" t="s">
+      <c r="A36" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B36" s="25" t="s">
         <v>41</v>
       </c>
-      <c r="C36" s="54"/>
-      <c r="D36" s="51" t="s">
+      <c r="C36" s="26"/>
+      <c r="D36" s="90" t="s">
         <v>101</v>
       </c>
-      <c r="E36" s="15"/>
-      <c r="F36" s="15"/>
-      <c r="G36" s="15"/>
-      <c r="H36" s="15"/>
-      <c r="I36" s="15"/>
-      <c r="J36" s="16"/>
+      <c r="E36" s="91"/>
+      <c r="F36" s="91"/>
+      <c r="G36" s="91"/>
+      <c r="H36" s="91"/>
+      <c r="I36" s="91"/>
+      <c r="J36" s="92"/>
       <c r="K36" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="L36" s="28" t="s">
+      <c r="L36" s="58" t="s">
         <v>109</v>
       </c>
-      <c r="M36" s="28"/>
-      <c r="N36" s="28"/>
-      <c r="O36" s="54"/>
+      <c r="M36" s="58"/>
+      <c r="N36" s="58"/>
+      <c r="O36" s="59"/>
     </row>
     <row r="37" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="B37" s="28" t="s">
+      <c r="A37" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B37" s="25" t="s">
         <v>27</v>
       </c>
-      <c r="C37" s="54"/>
-      <c r="D37" s="62"/>
-      <c r="E37" s="63"/>
-      <c r="F37" s="63"/>
-      <c r="G37" s="63"/>
-      <c r="H37" s="63"/>
-      <c r="I37" s="63"/>
-      <c r="J37" s="64"/>
+      <c r="C37" s="26"/>
+      <c r="D37" s="48"/>
+      <c r="E37" s="49"/>
+      <c r="F37" s="49"/>
+      <c r="G37" s="49"/>
+      <c r="H37" s="49"/>
+      <c r="I37" s="49"/>
+      <c r="J37" s="50"/>
       <c r="K37" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="L37" s="28" t="s">
+      <c r="L37" s="58" t="s">
         <v>104</v>
       </c>
-      <c r="M37" s="28"/>
-      <c r="N37" s="28"/>
-      <c r="O37" s="54"/>
+      <c r="M37" s="58"/>
+      <c r="N37" s="58"/>
+      <c r="O37" s="59"/>
     </row>
     <row r="38" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="B38" s="28" t="s">
+      <c r="A38" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B38" s="25" t="s">
         <v>28</v>
       </c>
-      <c r="C38" s="54"/>
-      <c r="D38" s="62"/>
-      <c r="E38" s="63"/>
-      <c r="F38" s="63"/>
-      <c r="G38" s="63"/>
-      <c r="H38" s="63"/>
-      <c r="I38" s="63"/>
-      <c r="J38" s="64"/>
+      <c r="C38" s="26"/>
+      <c r="D38" s="48"/>
+      <c r="E38" s="49"/>
+      <c r="F38" s="49"/>
+      <c r="G38" s="49"/>
+      <c r="H38" s="49"/>
+      <c r="I38" s="49"/>
+      <c r="J38" s="50"/>
       <c r="K38" s="57" t="s">
         <v>54</v>
       </c>
-      <c r="L38" s="28" t="s">
+      <c r="L38" s="58" t="s">
         <v>110</v>
       </c>
-      <c r="M38" s="28"/>
-      <c r="N38" s="28"/>
-      <c r="O38" s="54"/>
+      <c r="M38" s="58"/>
+      <c r="N38" s="58"/>
+      <c r="O38" s="59"/>
     </row>
     <row r="39" spans="1:15" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="B39" s="28" t="s">
+      <c r="A39" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B39" s="25" t="s">
         <v>29</v>
       </c>
-      <c r="C39" s="54"/>
-      <c r="D39" s="24"/>
-      <c r="E39" s="26"/>
-      <c r="F39" s="26"/>
-      <c r="G39" s="26"/>
-      <c r="H39" s="26"/>
-      <c r="I39" s="26"/>
-      <c r="J39" s="25"/>
-      <c r="K39" s="59" t="s">
-        <v>54</v>
-      </c>
-      <c r="L39" s="60" t="s">
+      <c r="C39" s="26"/>
+      <c r="D39" s="51"/>
+      <c r="E39" s="52"/>
+      <c r="F39" s="52"/>
+      <c r="G39" s="52"/>
+      <c r="H39" s="52"/>
+      <c r="I39" s="52"/>
+      <c r="J39" s="53"/>
+      <c r="K39" s="64" t="s">
+        <v>54</v>
+      </c>
+      <c r="L39" s="61" t="s">
         <v>105</v>
       </c>
-      <c r="M39" s="60"/>
-      <c r="N39" s="60"/>
-      <c r="O39" s="61"/>
+      <c r="M39" s="61"/>
+      <c r="N39" s="61"/>
+      <c r="O39" s="62"/>
     </row>
     <row r="40" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="B40" s="28" t="s">
+      <c r="A40" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B40" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="C40" s="54"/>
-      <c r="D40" s="66" t="s">
+      <c r="C40" s="26"/>
+      <c r="D40" s="102" t="s">
         <v>127</v>
       </c>
-      <c r="E40" s="67"/>
-      <c r="F40" s="67"/>
-      <c r="G40" s="67"/>
-      <c r="H40" s="67"/>
-      <c r="I40" s="67"/>
-      <c r="J40" s="67"/>
-      <c r="K40" s="67"/>
-      <c r="L40" s="67"/>
-      <c r="M40" s="67"/>
-      <c r="N40" s="67"/>
-      <c r="O40" s="68"/>
+      <c r="E40" s="103"/>
+      <c r="F40" s="103"/>
+      <c r="G40" s="103"/>
+      <c r="H40" s="103"/>
+      <c r="I40" s="103"/>
+      <c r="J40" s="103"/>
+      <c r="K40" s="103"/>
+      <c r="L40" s="103"/>
+      <c r="M40" s="103"/>
+      <c r="N40" s="103"/>
+      <c r="O40" s="104"/>
     </row>
     <row r="41" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="B41" s="28" t="s">
+      <c r="A41" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B41" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="C41" s="54"/>
-      <c r="D41" s="69"/>
-      <c r="E41" s="70"/>
-      <c r="F41" s="70"/>
-      <c r="G41" s="70"/>
-      <c r="H41" s="70"/>
-      <c r="I41" s="70"/>
-      <c r="J41" s="70"/>
-      <c r="K41" s="70"/>
-      <c r="L41" s="70"/>
-      <c r="M41" s="70"/>
-      <c r="N41" s="70"/>
-      <c r="O41" s="71"/>
+      <c r="C41" s="26"/>
+      <c r="D41" s="105"/>
+      <c r="E41" s="106"/>
+      <c r="F41" s="106"/>
+      <c r="G41" s="106"/>
+      <c r="H41" s="106"/>
+      <c r="I41" s="106"/>
+      <c r="J41" s="106"/>
+      <c r="K41" s="106"/>
+      <c r="L41" s="106"/>
+      <c r="M41" s="106"/>
+      <c r="N41" s="106"/>
+      <c r="O41" s="107"/>
     </row>
     <row r="42" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A42" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="B42" s="28" t="s">
+      <c r="A42" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B42" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="C42" s="54"/>
-      <c r="D42" s="62"/>
-      <c r="E42" s="63"/>
-      <c r="F42" s="63"/>
-      <c r="G42" s="63"/>
-      <c r="H42" s="63"/>
-      <c r="I42" s="63"/>
-      <c r="J42" s="63"/>
-      <c r="K42" s="63"/>
-      <c r="L42" s="63"/>
-      <c r="M42" s="63"/>
-      <c r="N42" s="63"/>
-      <c r="O42" s="64"/>
+      <c r="C42" s="26"/>
+      <c r="D42" s="96"/>
+      <c r="E42" s="97"/>
+      <c r="F42" s="97"/>
+      <c r="G42" s="97"/>
+      <c r="H42" s="97"/>
+      <c r="I42" s="97"/>
+      <c r="J42" s="97"/>
+      <c r="K42" s="97"/>
+      <c r="L42" s="97"/>
+      <c r="M42" s="97"/>
+      <c r="N42" s="97"/>
+      <c r="O42" s="98"/>
     </row>
     <row r="43" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="B43" s="28" t="s">
+      <c r="A43" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B43" s="25" t="s">
         <v>33</v>
       </c>
-      <c r="C43" s="54"/>
-      <c r="D43" s="62"/>
-      <c r="E43" s="63"/>
-      <c r="F43" s="63"/>
-      <c r="G43" s="63"/>
-      <c r="H43" s="63"/>
-      <c r="I43" s="63"/>
-      <c r="J43" s="63"/>
-      <c r="K43" s="63"/>
-      <c r="L43" s="63"/>
-      <c r="M43" s="63"/>
-      <c r="N43" s="63"/>
-      <c r="O43" s="64"/>
+      <c r="C43" s="26"/>
+      <c r="D43" s="96"/>
+      <c r="E43" s="97"/>
+      <c r="F43" s="97"/>
+      <c r="G43" s="97"/>
+      <c r="H43" s="97"/>
+      <c r="I43" s="97"/>
+      <c r="J43" s="97"/>
+      <c r="K43" s="97"/>
+      <c r="L43" s="97"/>
+      <c r="M43" s="97"/>
+      <c r="N43" s="97"/>
+      <c r="O43" s="98"/>
     </row>
     <row r="44" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="B44" s="28" t="s">
+      <c r="A44" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B44" s="25" t="s">
         <v>34</v>
       </c>
-      <c r="C44" s="54"/>
-      <c r="D44" s="62"/>
-      <c r="E44" s="63"/>
-      <c r="F44" s="63"/>
-      <c r="G44" s="63"/>
-      <c r="H44" s="63"/>
-      <c r="I44" s="63"/>
-      <c r="J44" s="63"/>
-      <c r="K44" s="63"/>
-      <c r="L44" s="63"/>
-      <c r="M44" s="63"/>
-      <c r="N44" s="63"/>
-      <c r="O44" s="64"/>
+      <c r="C44" s="26"/>
+      <c r="D44" s="96"/>
+      <c r="E44" s="97"/>
+      <c r="F44" s="97"/>
+      <c r="G44" s="97"/>
+      <c r="H44" s="97"/>
+      <c r="I44" s="97"/>
+      <c r="J44" s="97"/>
+      <c r="K44" s="97"/>
+      <c r="L44" s="97"/>
+      <c r="M44" s="97"/>
+      <c r="N44" s="97"/>
+      <c r="O44" s="98"/>
     </row>
     <row r="45" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A45" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="B45" s="28" t="s">
+      <c r="A45" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B45" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="C45" s="54"/>
-      <c r="D45" s="62"/>
-      <c r="E45" s="63"/>
-      <c r="F45" s="63"/>
-      <c r="G45" s="63"/>
-      <c r="H45" s="63"/>
-      <c r="I45" s="63"/>
-      <c r="J45" s="63"/>
-      <c r="K45" s="63"/>
-      <c r="L45" s="63"/>
-      <c r="M45" s="63"/>
-      <c r="N45" s="63"/>
-      <c r="O45" s="64"/>
+      <c r="C45" s="26"/>
+      <c r="D45" s="96"/>
+      <c r="E45" s="97"/>
+      <c r="F45" s="97"/>
+      <c r="G45" s="97"/>
+      <c r="H45" s="97"/>
+      <c r="I45" s="97"/>
+      <c r="J45" s="97"/>
+      <c r="K45" s="97"/>
+      <c r="L45" s="97"/>
+      <c r="M45" s="97"/>
+      <c r="N45" s="97"/>
+      <c r="O45" s="98"/>
     </row>
     <row r="46" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="B46" s="28" t="s">
+      <c r="A46" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B46" s="25" t="s">
         <v>36</v>
       </c>
-      <c r="C46" s="54"/>
-      <c r="D46" s="62"/>
-      <c r="E46" s="63"/>
-      <c r="F46" s="63"/>
-      <c r="G46" s="63"/>
-      <c r="H46" s="63"/>
-      <c r="I46" s="63"/>
-      <c r="J46" s="63"/>
-      <c r="K46" s="63"/>
-      <c r="L46" s="63"/>
-      <c r="M46" s="63"/>
-      <c r="N46" s="63"/>
-      <c r="O46" s="64"/>
+      <c r="C46" s="26"/>
+      <c r="D46" s="96"/>
+      <c r="E46" s="97"/>
+      <c r="F46" s="97"/>
+      <c r="G46" s="97"/>
+      <c r="H46" s="97"/>
+      <c r="I46" s="97"/>
+      <c r="J46" s="97"/>
+      <c r="K46" s="97"/>
+      <c r="L46" s="97"/>
+      <c r="M46" s="97"/>
+      <c r="N46" s="97"/>
+      <c r="O46" s="98"/>
     </row>
     <row r="47" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="56" t="s">
-        <v>54</v>
-      </c>
-      <c r="B47" s="28" t="s">
+      <c r="A47" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="B47" s="25" t="s">
         <v>37</v>
       </c>
-      <c r="C47" s="54"/>
-      <c r="D47" s="62"/>
-      <c r="E47" s="63"/>
-      <c r="F47" s="63"/>
-      <c r="G47" s="63"/>
-      <c r="H47" s="63"/>
-      <c r="I47" s="63"/>
-      <c r="J47" s="63"/>
-      <c r="K47" s="63"/>
-      <c r="L47" s="63"/>
-      <c r="M47" s="63"/>
-      <c r="N47" s="63"/>
-      <c r="O47" s="64"/>
+      <c r="C47" s="26"/>
+      <c r="D47" s="96"/>
+      <c r="E47" s="97"/>
+      <c r="F47" s="97"/>
+      <c r="G47" s="97"/>
+      <c r="H47" s="97"/>
+      <c r="I47" s="97"/>
+      <c r="J47" s="97"/>
+      <c r="K47" s="97"/>
+      <c r="L47" s="97"/>
+      <c r="M47" s="97"/>
+      <c r="N47" s="97"/>
+      <c r="O47" s="98"/>
     </row>
     <row r="48" spans="1:15" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A48" s="40" t="s">
-        <v>54</v>
-      </c>
-      <c r="B48" s="60" t="s">
+      <c r="A48" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="B48" s="29" t="s">
         <v>38</v>
       </c>
-      <c r="C48" s="61"/>
-      <c r="D48" s="24"/>
-      <c r="E48" s="26"/>
-      <c r="F48" s="26"/>
-      <c r="G48" s="26"/>
-      <c r="H48" s="26"/>
-      <c r="I48" s="26"/>
-      <c r="J48" s="26"/>
-      <c r="K48" s="26"/>
-      <c r="L48" s="26"/>
-      <c r="M48" s="26"/>
-      <c r="N48" s="26"/>
-      <c r="O48" s="25"/>
+      <c r="C48" s="30"/>
+      <c r="D48" s="99"/>
+      <c r="E48" s="100"/>
+      <c r="F48" s="100"/>
+      <c r="G48" s="100"/>
+      <c r="H48" s="100"/>
+      <c r="I48" s="100"/>
+      <c r="J48" s="100"/>
+      <c r="K48" s="100"/>
+      <c r="L48" s="100"/>
+      <c r="M48" s="100"/>
+      <c r="N48" s="100"/>
+      <c r="O48" s="101"/>
     </row>
   </sheetData>
   <mergeCells count="37">

</xml_diff>